<commit_message>
Added Amplifiers, Comms, & Conversion ICs
Also fixed some packages' name layer
</commit_message>
<xml_diff>
--- a/CougsInSpace-Inventory.xlsx
+++ b/CougsInSpace-Inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bradley\Documents\CougsInSpace\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9DCD98-80F2-4A14-9064-C7EF114D46A3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9D258F-179D-40C5-B78A-7CE9FCF2B712}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="5" xr2:uid="{42A108CB-A0BE-49ED-8B7A-3FB1AB856735}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="6" xr2:uid="{42A108CB-A0BE-49ED-8B7A-3FB1AB856735}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3377" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3392" uniqueCount="523">
   <si>
     <t>Vendors have been selected by high reputability and lowest price</t>
   </si>
@@ -1386,9 +1386,6 @@
   </si>
   <si>
     <t>02-0001</t>
-  </si>
-  <si>
-    <t>20-xxxx:Resistors</t>
   </si>
   <si>
     <t>40-xxxx: Crystal SMD</t>
@@ -1562,6 +1559,51 @@
   </si>
   <si>
     <t>51-0002</t>
+  </si>
+  <si>
+    <t>06-xxxx: Fuses SMD</t>
+  </si>
+  <si>
+    <t>07-xxxx: Fuses THT</t>
+  </si>
+  <si>
+    <t>48-xxxx: Hardware</t>
+  </si>
+  <si>
+    <t>49-xxxx: Electromechanical</t>
+  </si>
+  <si>
+    <t>08-xxxx: Amplifiers (excluding RF)</t>
+  </si>
+  <si>
+    <t>09-xxxx: Communication ICs</t>
+  </si>
+  <si>
+    <t>26-xxxx: All other resistors</t>
+  </si>
+  <si>
+    <t>27-xxxx: Conversion Ics</t>
+  </si>
+  <si>
+    <t>20-xxxx: Resistor 1005 (0402 in)</t>
+  </si>
+  <si>
+    <t>21-xxxx: Resistor 1608 (0603 in)</t>
+  </si>
+  <si>
+    <t>22-xxxx: Resistor 2012 (0805 in)</t>
+  </si>
+  <si>
+    <t>23-xxxx: Resistor 3216 (1206 in)</t>
+  </si>
+  <si>
+    <t>24-xxxx: Resistor 3225 (1210 in) and larger</t>
+  </si>
+  <si>
+    <t>25-xxxx: Resistor THT</t>
+  </si>
+  <si>
+    <t>27-0001</t>
   </si>
 </sst>
 </file>
@@ -1654,7 +1696,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1687,6 +1729,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2076,12 +2119,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5382E235-B063-4394-927B-0549E269B25A}">
-  <dimension ref="A1:J165"/>
+  <dimension ref="A1:J164"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="10" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2091,10 +2134,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="24"/>
       <c r="C1" s="1"/>
       <c r="D1" s="21"/>
       <c r="E1" s="1"/>
@@ -2103,10 +2146,10 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="24"/>
+      <c r="B2" s="25"/>
       <c r="C2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="2"/>
@@ -2116,18 +2159,18 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="25"/>
+      <c r="B3" s="26"/>
       <c r="C3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="7"/>
       <c r="E4" s="7"/>
     </row>
@@ -2186,7 +2229,7 @@
     </row>
     <row r="14" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2206,830 +2249,845 @@
     </row>
     <row r="18" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>478</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>411</v>
+      </c>
+      <c r="B24" s="27"/>
+    </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
-        <v>411</v>
-      </c>
-      <c r="B25" s="26"/>
+      <c r="A25" s="27" t="s">
+        <v>412</v>
+      </c>
+      <c r="B25" s="27"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
-        <v>412</v>
-      </c>
-      <c r="B26" s="26"/>
+      <c r="A26" s="27" t="s">
+        <v>413</v>
+      </c>
+      <c r="B26" s="27"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
-        <v>413</v>
-      </c>
-      <c r="B27" s="26"/>
+      <c r="A27" s="27" t="s">
+        <v>414</v>
+      </c>
+      <c r="B27" s="27"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
-        <v>414</v>
-      </c>
-      <c r="B28" s="26"/>
+      <c r="A28" s="27" t="s">
+        <v>415</v>
+      </c>
+      <c r="B28" s="27"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
-        <v>415</v>
-      </c>
-      <c r="B29" s="26"/>
+      <c r="A29" s="27" t="s">
+        <v>416</v>
+      </c>
+      <c r="B29" s="27"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
-        <v>416</v>
-      </c>
-      <c r="B30" s="26"/>
+      <c r="A30" s="27" t="s">
+        <v>417</v>
+      </c>
+      <c r="B30" s="27"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
-        <v>417</v>
-      </c>
-      <c r="B31" s="26"/>
+      <c r="A31" s="27" t="s">
+        <v>418</v>
+      </c>
+      <c r="B31" s="27"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
-        <v>418</v>
-      </c>
-      <c r="B32" s="26"/>
+      <c r="A32" s="27" t="s">
+        <v>419</v>
+      </c>
+      <c r="B32" s="27"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
-        <v>419</v>
-      </c>
-      <c r="B33" s="26"/>
+      <c r="A33" s="27" t="s">
+        <v>420</v>
+      </c>
+      <c r="B33" s="27"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
-        <v>420</v>
-      </c>
-      <c r="B34" s="26"/>
+      <c r="A34" s="28" t="s">
+        <v>516</v>
+      </c>
+      <c r="B34" s="28"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
+        <v>517</v>
+      </c>
+      <c r="B35" s="27"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
+        <v>518</v>
+      </c>
+      <c r="B36" s="27"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>519</v>
+      </c>
+      <c r="B37" s="27"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="B38" s="28"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="28" t="s">
+        <v>521</v>
+      </c>
+      <c r="B39" s="28"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="28" t="s">
+        <v>514</v>
+      </c>
+      <c r="B40" s="28"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="28" t="s">
+        <v>515</v>
+      </c>
+      <c r="B41" s="28"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="28">
+        <v>28</v>
+      </c>
+      <c r="B42" s="28"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="28">
+        <v>29</v>
+      </c>
+      <c r="B43" s="28"/>
+    </row>
+    <row r="44" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="29" t="s">
+        <v>471</v>
+      </c>
+      <c r="B44" s="29"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="27" t="s">
+        <v>462</v>
+      </c>
+      <c r="B45" s="27"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="27" t="s">
+        <v>463</v>
+      </c>
+      <c r="B46" s="27"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="27" t="s">
+        <v>464</v>
+      </c>
+      <c r="B47" s="27"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="27" t="s">
+        <v>465</v>
+      </c>
+      <c r="B48" s="27"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="27" t="s">
+        <v>466</v>
+      </c>
+      <c r="B49" s="27"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="27" t="s">
+        <v>467</v>
+      </c>
+      <c r="B50" s="27"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="27" t="s">
+        <v>468</v>
+      </c>
+      <c r="B51" s="27"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="27" t="s">
+        <v>469</v>
+      </c>
+      <c r="B52" s="27"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="27" t="s">
+        <v>470</v>
+      </c>
+      <c r="B53" s="27"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="27" t="s">
         <v>451</v>
       </c>
-      <c r="B35" s="27"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="26">
-        <v>21</v>
-      </c>
-      <c r="B36" s="26"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="26">
-        <v>22</v>
-      </c>
-      <c r="B37" s="26"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="26">
-        <v>23</v>
-      </c>
-      <c r="B38" s="26"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="27">
-        <v>24</v>
-      </c>
-      <c r="B39" s="27"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="27">
-        <v>25</v>
-      </c>
-      <c r="B40" s="27"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="27">
-        <v>26</v>
-      </c>
-      <c r="B41" s="27"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="27">
-        <v>27</v>
-      </c>
-      <c r="B42" s="27"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="27">
-        <v>28</v>
-      </c>
-      <c r="B43" s="27"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="27">
-        <v>29</v>
-      </c>
-      <c r="B44" s="27"/>
-    </row>
-    <row r="45" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="s">
-        <v>472</v>
-      </c>
-      <c r="B45" s="28"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
-        <v>463</v>
-      </c>
-      <c r="B46" s="26"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="s">
-        <v>464</v>
-      </c>
-      <c r="B47" s="26"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
-        <v>465</v>
-      </c>
-      <c r="B48" s="26"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="26" t="s">
-        <v>466</v>
-      </c>
-      <c r="B49" s="26"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="26" t="s">
-        <v>467</v>
-      </c>
-      <c r="B50" s="26"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="26" t="s">
-        <v>468</v>
-      </c>
-      <c r="B51" s="26"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="26" t="s">
-        <v>469</v>
-      </c>
-      <c r="B52" s="26"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="26" t="s">
-        <v>470</v>
-      </c>
-      <c r="B53" s="26"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="s">
-        <v>471</v>
-      </c>
-      <c r="B54" s="26"/>
+      <c r="B54" s="27"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="26" t="s">
+      <c r="A55" s="27" t="s">
         <v>452</v>
       </c>
-      <c r="B55" s="26"/>
+      <c r="B55" s="27"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="26" t="s">
+      <c r="A56" s="27" t="s">
         <v>453</v>
       </c>
-      <c r="B56" s="26"/>
+      <c r="B56" s="27"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="26" t="s">
+      <c r="A57" s="28" t="s">
         <v>454</v>
       </c>
-      <c r="B57" s="26"/>
+      <c r="B57" s="28"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="27" t="s">
+      <c r="A58" s="28" t="s">
         <v>455</v>
       </c>
-      <c r="B58" s="27"/>
+      <c r="B58" s="28"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="27" t="s">
+      <c r="A59" s="28" t="s">
         <v>456</v>
       </c>
-      <c r="B59" s="27"/>
+      <c r="B59" s="28"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="27" t="s">
+      <c r="A60" s="28" t="s">
         <v>457</v>
       </c>
-      <c r="B60" s="27"/>
+      <c r="B60" s="28"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="27" t="s">
+      <c r="A61" s="28" t="s">
         <v>458</v>
       </c>
-      <c r="B61" s="27"/>
+      <c r="B61" s="28"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="27" t="s">
-        <v>459</v>
+        <v>510</v>
       </c>
       <c r="B62" s="27"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="26">
-        <v>48</v>
-      </c>
-      <c r="B63" s="26"/>
+      <c r="A63" s="27" t="s">
+        <v>511</v>
+      </c>
+      <c r="B63" s="27"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="26">
-        <v>49</v>
-      </c>
-      <c r="B64" s="26"/>
+      <c r="A64" s="27" t="s">
+        <v>488</v>
+      </c>
+      <c r="B64" s="27"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="26" t="s">
+      <c r="A65" s="27" t="s">
         <v>489</v>
       </c>
-      <c r="B65" s="26"/>
+      <c r="B65" s="27"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="26" t="s">
+      <c r="A66" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="B66" s="26"/>
+      <c r="B66" s="27"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="26" t="s">
+      <c r="A67" s="27" t="s">
         <v>491</v>
       </c>
-      <c r="B67" s="26"/>
+      <c r="B67" s="27"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="26" t="s">
+      <c r="A68" s="27" t="s">
         <v>492</v>
       </c>
-      <c r="B68" s="26"/>
+      <c r="B68" s="27"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="26" t="s">
+      <c r="A69" s="27" t="s">
         <v>493</v>
       </c>
-      <c r="B69" s="26"/>
+      <c r="B69" s="27"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="26" t="s">
+      <c r="A70" s="27" t="s">
         <v>494</v>
       </c>
-      <c r="B70" s="26"/>
+      <c r="B70" s="27"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="26" t="s">
+      <c r="A71" s="27" t="s">
         <v>495</v>
       </c>
-      <c r="B71" s="26"/>
+      <c r="B71" s="27"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="26" t="s">
+      <c r="A72" s="27" t="s">
         <v>496</v>
       </c>
-      <c r="B72" s="26"/>
+      <c r="B72" s="27"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="26" t="s">
+      <c r="A73" s="27" t="s">
         <v>497</v>
       </c>
-      <c r="B73" s="26"/>
+      <c r="B73" s="27"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="26" t="s">
-        <v>498</v>
-      </c>
-      <c r="B74" s="26"/>
+      <c r="A74" s="27"/>
+      <c r="B74" s="27"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="26"/>
-      <c r="B75" s="26"/>
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="26"/>
-      <c r="B76" s="26"/>
+      <c r="A76" s="27"/>
+      <c r="B76" s="27"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="26"/>
-      <c r="B77" s="26"/>
+      <c r="A77" s="27"/>
+      <c r="B77" s="27"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="26"/>
-      <c r="B78" s="26"/>
+      <c r="A78" s="27"/>
+      <c r="B78" s="27"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="26"/>
-      <c r="B79" s="26"/>
+      <c r="A79" s="27"/>
+      <c r="B79" s="27"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="26"/>
-      <c r="B80" s="26"/>
+      <c r="A80" s="27"/>
+      <c r="B80" s="27"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="26"/>
-      <c r="B81" s="26"/>
+      <c r="A81" s="27"/>
+      <c r="B81" s="27"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="26"/>
-      <c r="B82" s="26"/>
+      <c r="A82" s="27"/>
+      <c r="B82" s="27"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="26"/>
-      <c r="B83" s="26"/>
+      <c r="A83" s="27"/>
+      <c r="B83" s="27"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="26"/>
-      <c r="B84" s="26"/>
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="26"/>
-      <c r="B85" s="26"/>
+      <c r="A85" s="27"/>
+      <c r="B85" s="27"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="26"/>
-      <c r="B86" s="26"/>
+      <c r="A86" s="27"/>
+      <c r="B86" s="27"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="26"/>
-      <c r="B87" s="26"/>
+      <c r="A87" s="27"/>
+      <c r="B87" s="27"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="26"/>
-      <c r="B88" s="26"/>
+      <c r="A88" s="27"/>
+      <c r="B88" s="27"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="26"/>
-      <c r="B89" s="26"/>
+      <c r="A89" s="27"/>
+      <c r="B89" s="27"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="26"/>
-      <c r="B90" s="26"/>
+      <c r="A90" s="27"/>
+      <c r="B90" s="27"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="26"/>
-      <c r="B91" s="26"/>
+      <c r="A91" s="27"/>
+      <c r="B91" s="27"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="26"/>
-      <c r="B92" s="26"/>
+      <c r="A92" s="27"/>
+      <c r="B92" s="27"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="26"/>
-      <c r="B93" s="26"/>
+      <c r="A93" s="27"/>
+      <c r="B93" s="27"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="26"/>
-      <c r="B94" s="26"/>
+      <c r="A94" s="27"/>
+      <c r="B94" s="27"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="26"/>
-      <c r="B95" s="26"/>
+      <c r="A95" s="27"/>
+      <c r="B95" s="27"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="26"/>
-      <c r="B96" s="26"/>
+      <c r="A96" s="27"/>
+      <c r="B96" s="27"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="26"/>
-      <c r="B97" s="26"/>
+      <c r="A97" s="27"/>
+      <c r="B97" s="27"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="26"/>
-      <c r="B98" s="26"/>
+      <c r="A98" s="27"/>
+      <c r="B98" s="27"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="26"/>
-      <c r="B99" s="26"/>
+      <c r="A99" s="27"/>
+      <c r="B99" s="27"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="26"/>
-      <c r="B100" s="26"/>
+      <c r="A100" s="27"/>
+      <c r="B100" s="27"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="26"/>
-      <c r="B101" s="26"/>
+      <c r="A101" s="27"/>
+      <c r="B101" s="27"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="26"/>
-      <c r="B102" s="26"/>
+      <c r="A102" s="27"/>
+      <c r="B102" s="27"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="26"/>
-      <c r="B103" s="26"/>
+      <c r="A103" s="27"/>
+      <c r="B103" s="27"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="26"/>
-      <c r="B104" s="26"/>
+      <c r="A104" s="27"/>
+      <c r="B104" s="27"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="26"/>
-      <c r="B105" s="26"/>
+      <c r="A105" s="27"/>
+      <c r="B105" s="27"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="26"/>
-      <c r="B106" s="26"/>
+      <c r="A106" s="27"/>
+      <c r="B106" s="27"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="26"/>
-      <c r="B107" s="26"/>
+      <c r="A107" s="27"/>
+      <c r="B107" s="27"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="26"/>
-      <c r="B108" s="26"/>
+      <c r="A108" s="27"/>
+      <c r="B108" s="27"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="26"/>
-      <c r="B109" s="26"/>
+      <c r="A109" s="27"/>
+      <c r="B109" s="27"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="26"/>
-      <c r="B110" s="26"/>
+      <c r="A110" s="27"/>
+      <c r="B110" s="27"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="26"/>
-      <c r="B111" s="26"/>
+      <c r="A111" s="27"/>
+      <c r="B111" s="27"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="26"/>
-      <c r="B112" s="26"/>
+      <c r="A112" s="27"/>
+      <c r="B112" s="27"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="26"/>
-      <c r="B113" s="26"/>
+      <c r="A113" s="27"/>
+      <c r="B113" s="27"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="26"/>
-      <c r="B114" s="26"/>
+      <c r="A114" s="27"/>
+      <c r="B114" s="27"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="26"/>
-      <c r="B115" s="26"/>
+      <c r="A115" s="27"/>
+      <c r="B115" s="27"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="26"/>
-      <c r="B116" s="26"/>
+      <c r="A116" s="27"/>
+      <c r="B116" s="27"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="26"/>
-      <c r="B117" s="26"/>
+      <c r="A117" s="27"/>
+      <c r="B117" s="27"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="26"/>
-      <c r="B118" s="26"/>
+      <c r="A118" s="27"/>
+      <c r="B118" s="27"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="26"/>
-      <c r="B119" s="26"/>
+      <c r="A119" s="27"/>
+      <c r="B119" s="27"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="26"/>
-      <c r="B120" s="26"/>
+      <c r="A120" s="27"/>
+      <c r="B120" s="27"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="26"/>
-      <c r="B121" s="26"/>
+      <c r="A121" s="27"/>
+      <c r="B121" s="27"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="26"/>
-      <c r="B122" s="26"/>
+      <c r="A122" s="27"/>
+      <c r="B122" s="27"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="26"/>
-      <c r="B123" s="26"/>
+      <c r="A123" s="27"/>
+      <c r="B123" s="27"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="26"/>
-      <c r="B124" s="26"/>
+      <c r="A124" s="27"/>
+      <c r="B124" s="27"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="26"/>
-      <c r="B125" s="26"/>
+      <c r="A125" s="27"/>
+      <c r="B125" s="27"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="26"/>
-      <c r="B126" s="26"/>
+      <c r="A126" s="27"/>
+      <c r="B126" s="27"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="26"/>
-      <c r="B127" s="26"/>
+      <c r="A127" s="27"/>
+      <c r="B127" s="27"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="26"/>
-      <c r="B128" s="26"/>
+      <c r="A128" s="27"/>
+      <c r="B128" s="27"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="26"/>
-      <c r="B129" s="26"/>
+      <c r="A129" s="27"/>
+      <c r="B129" s="27"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="26"/>
-      <c r="B130" s="26"/>
+      <c r="A130" s="27"/>
+      <c r="B130" s="27"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="26"/>
-      <c r="B131" s="26"/>
+      <c r="A131" s="27"/>
+      <c r="B131" s="27"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="26"/>
-      <c r="B132" s="26"/>
+      <c r="A132" s="27"/>
+      <c r="B132" s="27"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="26"/>
-      <c r="B133" s="26"/>
+      <c r="A133" s="27"/>
+      <c r="B133" s="27"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="26"/>
-      <c r="B134" s="26"/>
+      <c r="A134" s="27"/>
+      <c r="B134" s="27"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="26"/>
-      <c r="B135" s="26"/>
+      <c r="A135" s="27"/>
+      <c r="B135" s="27"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="26"/>
-      <c r="B136" s="26"/>
+      <c r="A136" s="27"/>
+      <c r="B136" s="27"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="26"/>
-      <c r="B137" s="26"/>
+      <c r="A137" s="27"/>
+      <c r="B137" s="27"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="26"/>
-      <c r="B138" s="26"/>
+      <c r="A138" s="27"/>
+      <c r="B138" s="27"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="26"/>
-      <c r="B139" s="26"/>
+      <c r="A139" s="27"/>
+      <c r="B139" s="27"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="26"/>
-      <c r="B140" s="26"/>
+      <c r="A140" s="27"/>
+      <c r="B140" s="27"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="26"/>
-      <c r="B141" s="26"/>
+      <c r="A141" s="27"/>
+      <c r="B141" s="27"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="26"/>
-      <c r="B142" s="26"/>
+      <c r="A142" s="27"/>
+      <c r="B142" s="27"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="26"/>
-      <c r="B143" s="26"/>
+      <c r="A143" s="27"/>
+      <c r="B143" s="27"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="26"/>
-      <c r="B144" s="26"/>
+      <c r="A144" s="27"/>
+      <c r="B144" s="27"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="26"/>
-      <c r="B145" s="26"/>
+      <c r="A145" s="27"/>
+      <c r="B145" s="27"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="26"/>
-      <c r="B146" s="26"/>
+      <c r="A146" s="27"/>
+      <c r="B146" s="27"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="26"/>
-      <c r="B147" s="26"/>
+      <c r="A147" s="27"/>
+      <c r="B147" s="27"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="26"/>
-      <c r="B148" s="26"/>
+      <c r="A148" s="27"/>
+      <c r="B148" s="27"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="26"/>
-      <c r="B149" s="26"/>
+      <c r="A149" s="27"/>
+      <c r="B149" s="27"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="26"/>
-      <c r="B150" s="26"/>
+      <c r="A150" s="27"/>
+      <c r="B150" s="27"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="26"/>
-      <c r="B151" s="26"/>
+      <c r="A151" s="27"/>
+      <c r="B151" s="27"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="26"/>
-      <c r="B152" s="26"/>
+      <c r="A152" s="27"/>
+      <c r="B152" s="27"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="26"/>
-      <c r="B153" s="26"/>
+      <c r="A153" s="27"/>
+      <c r="B153" s="27"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="26"/>
-      <c r="B154" s="26"/>
+      <c r="A154" s="27"/>
+      <c r="B154" s="27"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="26"/>
-      <c r="B155" s="26"/>
+      <c r="A155" s="27"/>
+      <c r="B155" s="27"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="26"/>
-      <c r="B156" s="26"/>
+      <c r="A156" s="27"/>
+      <c r="B156" s="27"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="26"/>
-      <c r="B157" s="26"/>
+      <c r="A157" s="27"/>
+      <c r="B157" s="27"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="26"/>
-      <c r="B158" s="26"/>
+      <c r="A158" s="27"/>
+      <c r="B158" s="27"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="26"/>
-      <c r="B159" s="26"/>
+      <c r="A159" s="27"/>
+      <c r="B159" s="27"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="26"/>
-      <c r="B160" s="26"/>
+      <c r="A160" s="27"/>
+      <c r="B160" s="27"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="26"/>
-      <c r="B161" s="26"/>
+      <c r="A161" s="27"/>
+      <c r="B161" s="27"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="26"/>
-      <c r="B162" s="26"/>
+      <c r="A162" s="27"/>
+      <c r="B162" s="27"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="26"/>
-      <c r="B163" s="26"/>
+      <c r="A163" s="27"/>
+      <c r="B163" s="27"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="26"/>
-      <c r="B164" s="26"/>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="26"/>
-      <c r="B165" s="26"/>
+      <c r="A164" s="27"/>
+      <c r="B164" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="145">
+    <mergeCell ref="A160:B160"/>
     <mergeCell ref="A161:B161"/>
     <mergeCell ref="A162:B162"/>
     <mergeCell ref="A163:B163"/>
     <mergeCell ref="A164:B164"/>
-    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A155:B155"/>
     <mergeCell ref="A156:B156"/>
     <mergeCell ref="A157:B157"/>
     <mergeCell ref="A158:B158"/>
     <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A150:B150"/>
     <mergeCell ref="A151:B151"/>
     <mergeCell ref="A152:B152"/>
     <mergeCell ref="A153:B153"/>
     <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="A145:B145"/>
     <mergeCell ref="A146:B146"/>
     <mergeCell ref="A147:B147"/>
     <mergeCell ref="A148:B148"/>
     <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A140:B140"/>
     <mergeCell ref="A141:B141"/>
     <mergeCell ref="A142:B142"/>
     <mergeCell ref="A143:B143"/>
     <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A135:B135"/>
     <mergeCell ref="A136:B136"/>
     <mergeCell ref="A137:B137"/>
     <mergeCell ref="A138:B138"/>
     <mergeCell ref="A139:B139"/>
-    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A130:B130"/>
     <mergeCell ref="A131:B131"/>
     <mergeCell ref="A132:B132"/>
     <mergeCell ref="A133:B133"/>
     <mergeCell ref="A134:B134"/>
-    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A125:B125"/>
     <mergeCell ref="A126:B126"/>
     <mergeCell ref="A127:B127"/>
     <mergeCell ref="A128:B128"/>
     <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="A120:B120"/>
     <mergeCell ref="A121:B121"/>
     <mergeCell ref="A122:B122"/>
     <mergeCell ref="A123:B123"/>
     <mergeCell ref="A124:B124"/>
-    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A115:B115"/>
     <mergeCell ref="A116:B116"/>
     <mergeCell ref="A117:B117"/>
     <mergeCell ref="A118:B118"/>
     <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A110:B110"/>
     <mergeCell ref="A111:B111"/>
     <mergeCell ref="A112:B112"/>
     <mergeCell ref="A113:B113"/>
     <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A105:B105"/>
     <mergeCell ref="A106:B106"/>
     <mergeCell ref="A107:B107"/>
     <mergeCell ref="A108:B108"/>
     <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A100:B100"/>
     <mergeCell ref="A101:B101"/>
     <mergeCell ref="A102:B102"/>
     <mergeCell ref="A103:B103"/>
     <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A95:B95"/>
     <mergeCell ref="A96:B96"/>
     <mergeCell ref="A97:B97"/>
     <mergeCell ref="A98:B98"/>
     <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A90:B90"/>
     <mergeCell ref="A91:B91"/>
     <mergeCell ref="A92:B92"/>
     <mergeCell ref="A93:B93"/>
     <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A85:B85"/>
     <mergeCell ref="A86:B86"/>
     <mergeCell ref="A87:B87"/>
     <mergeCell ref="A88:B88"/>
     <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A80:B80"/>
     <mergeCell ref="A81:B81"/>
     <mergeCell ref="A82:B82"/>
     <mergeCell ref="A83:B83"/>
     <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A75:B75"/>
     <mergeCell ref="A76:B76"/>
     <mergeCell ref="A77:B77"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A70:B70"/>
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="A73:B73"/>
     <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A65:B65"/>
     <mergeCell ref="A66:B66"/>
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A68:B68"/>
     <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A61:B61"/>
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A55:B55"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A52:B52"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A45:B45"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A50:B50"/>
     <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A40:B40"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A30:B30"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3059,17 +3117,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
@@ -8610,16 +8668,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -10849,17 +10907,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -10907,7 +10965,7 @@
         <v>151</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>153</v>
@@ -10936,7 +10994,7 @@
         <v>152</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>155</v>
@@ -10965,7 +11023,7 @@
         <v>151</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>157</v>
@@ -10994,7 +11052,7 @@
         <v>1608</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>185</v>
@@ -11023,7 +11081,7 @@
         <v>151</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>233</v>
@@ -12531,17 +12589,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -12589,7 +12647,7 @@
         <v>168</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>183</v>
@@ -12618,7 +12676,7 @@
         <v>169</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>181</v>
@@ -12647,7 +12705,7 @@
         <v>168</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>180</v>
@@ -12676,7 +12734,7 @@
         <v>268</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>269</v>
@@ -12705,7 +12763,7 @@
         <v>337</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>338</v>
@@ -12734,7 +12792,7 @@
         <v>340</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G9" s="14">
         <v>5025700893</v>
@@ -12763,7 +12821,7 @@
         <v>346</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G10" s="15">
         <v>731000114</v>
@@ -12792,7 +12850,7 @@
         <v>337</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>351</v>
@@ -14266,7 +14324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2484DFB1-8EE9-471C-B790-EFC66E66E7FA}">
   <dimension ref="A1:I299"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -14285,17 +14343,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
@@ -14348,7 +14406,7 @@
         <v>164</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>172</v>
@@ -14377,7 +14435,7 @@
         <v>165</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>174</v>
@@ -14406,7 +14464,7 @@
         <v>167</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>178</v>
@@ -14435,7 +14493,7 @@
         <v>170</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>162</v>
@@ -14464,7 +14522,7 @@
         <v>171</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>188</v>
@@ -14493,7 +14551,7 @@
         <v>224</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>222</v>
@@ -14622,13 +14680,13 @@
         <v>0</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>506</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="22" t="s">
         <v>507</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>508</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>265</v>
@@ -14657,7 +14715,7 @@
         <v>170</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>274</v>
@@ -16104,10 +16162,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D526D2F0-6B58-44A3-8176-A7A0AAEF1CB8}">
-  <dimension ref="A1:H300"/>
+  <dimension ref="A1:I300"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16117,25 +16175,27 @@
     <col min="3" max="3" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="10"/>
+    <col min="6" max="6" width="14" style="23" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>108</v>
       </c>
@@ -16152,16 +16212,19 @@
         <v>4</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>8</v>
       </c>
@@ -16177,17 +16240,17 @@
       <c r="E4" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>12</v>
       </c>
@@ -16203,17 +16266,17 @@
       <c r="E5" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -16229,17 +16292,17 @@
       <c r="E6" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="I6" s="10" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -16255,17 +16318,17 @@
       <c r="E7" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="I7" s="10" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>9</v>
       </c>
@@ -16281,17 +16344,17 @@
       <c r="E8" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="I8" s="10" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>2</v>
       </c>
@@ -16307,17 +16370,17 @@
       <c r="E9" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="I9" s="10" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>3</v>
       </c>
@@ -16333,17 +16396,17 @@
       <c r="E10" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="I10" s="10" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>6</v>
       </c>
@@ -16359,17 +16422,17 @@
       <c r="E11" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="I11" s="10" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>4</v>
       </c>
@@ -16385,17 +16448,17 @@
       <c r="E12" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="I12" s="10" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>4</v>
       </c>
@@ -16411,17 +16474,17 @@
       <c r="E13" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="I13" s="10" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>4</v>
       </c>
@@ -16437,17 +16500,17 @@
       <c r="E14" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="H14" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="I14" s="10" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>12</v>
       </c>
@@ -16463,17 +16526,18 @@
       <c r="E15" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="5"/>
+      <c r="G15" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="I15" s="5" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>4</v>
       </c>
@@ -16489,17 +16553,17 @@
       <c r="E16" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="H16" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="I16" s="10" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>2</v>
       </c>
@@ -16515,17 +16579,17 @@
       <c r="E17" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="G17" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="H17" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="I17" s="10" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>4</v>
       </c>
@@ -16541,17 +16605,17 @@
       <c r="E18" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="H18" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="I18" s="10" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>1</v>
       </c>
@@ -16567,17 +16631,17 @@
       <c r="E19" s="10" t="s">
         <v>382</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="G19" s="10" t="s">
         <v>383</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="H19" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="I19" s="10" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>5</v>
       </c>
@@ -16593,17 +16657,17 @@
       <c r="E20" s="10" t="s">
         <v>386</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="G20" s="10" t="s">
         <v>387</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="H20" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="I20" s="10" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>5</v>
       </c>
@@ -16619,17 +16683,17 @@
       <c r="E21" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="G21" s="10" t="s">
         <v>389</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="H21" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="I21" s="10" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>0</v>
       </c>
@@ -16645,17 +16709,17 @@
       <c r="E22" s="10" t="s">
         <v>398</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="G22" s="10" t="s">
         <v>399</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="H22" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="I22" s="10" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>0</v>
       </c>
@@ -16671,57 +16735,60 @@
       <c r="E23" s="10" t="s">
         <v>402</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="23" t="s">
+        <v>522</v>
+      </c>
+      <c r="G23" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="H23" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="I23" s="10" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C31" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C32" s="2" t="s">
         <v>238</v>
       </c>
@@ -18068,7 +18135,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C300">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -18103,17 +18170,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -18188,7 +18255,7 @@
         <v>326</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>325</v>
@@ -18217,7 +18284,7 @@
         <v>349</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>348</v>
@@ -18293,7 +18360,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E9" s="5">
         <v>18650</v>
@@ -19808,20 +19875,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="17"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
       <c r="D2" s="18" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Added Sensors and a Logic IC
</commit_message>
<xml_diff>
--- a/CougsInSpace-Inventory.xlsx
+++ b/CougsInSpace-Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bradley\Documents\CougsInSpace\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A08AC1-AEFD-4EC2-9E96-6B0E213C26CC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC7AFFB-774E-4C3C-9AF6-70F2F1D6A1D5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="6" xr2:uid="{42A108CB-A0BE-49ED-8B7A-3FB1AB856735}"/>
   </bookViews>
@@ -1750,7 +1750,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1760,12 +1760,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1792,7 +1786,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1843,7 +1837,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -16279,8 +16272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D526D2F0-6B58-44A3-8176-A7A0AAEF1CB8}">
   <dimension ref="A1:I300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16355,7 +16348,7 @@
       <c r="E4" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="32" t="s">
         <v>537</v>
       </c>
       <c r="G4" s="10" t="s">
@@ -16413,7 +16406,7 @@
       <c r="E6" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="32" t="s">
         <v>541</v>
       </c>
       <c r="G6" s="10" t="s">
@@ -16442,7 +16435,7 @@
       <c r="E7" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="32" t="s">
         <v>542</v>
       </c>
       <c r="G7" s="10" t="s">
@@ -16500,7 +16493,7 @@
       <c r="E9" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="32" t="s">
         <v>543</v>
       </c>
       <c r="G9" s="10" t="s">
@@ -16558,7 +16551,7 @@
       <c r="E11" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="32" t="s">
         <v>538</v>
       </c>
       <c r="G11" s="10" t="s">
@@ -16587,7 +16580,7 @@
       <c r="E12" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="32" t="s">
         <v>539</v>
       </c>
       <c r="G12" s="5" t="s">
@@ -16616,7 +16609,7 @@
       <c r="E13" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="32" t="s">
         <v>544</v>
       </c>
       <c r="G13" s="5" t="s">
@@ -16645,7 +16638,7 @@
       <c r="E14" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="32" t="s">
         <v>545</v>
       </c>
       <c r="G14" s="10" t="s">
@@ -16703,7 +16696,7 @@
       <c r="E16" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="32" t="s">
         <v>546</v>
       </c>
       <c r="G16" s="5" t="s">
@@ -16732,7 +16725,7 @@
       <c r="E17" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="32" t="s">
         <v>547</v>
       </c>
       <c r="G17" s="10" t="s">
@@ -16790,7 +16783,7 @@
       <c r="E19" s="10" t="s">
         <v>382</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="32" t="s">
         <v>548</v>
       </c>
       <c r="G19" s="10" t="s">
@@ -16819,7 +16812,7 @@
       <c r="E20" s="10" t="s">
         <v>386</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="32" t="s">
         <v>549</v>
       </c>
       <c r="G20" s="10" t="s">

</xml_diff>

<commit_message>
Added Resistors, RF, LEDs, and Horizontal Symbols
</commit_message>
<xml_diff>
--- a/CougsInSpace-Inventory.xlsx
+++ b/CougsInSpace-Inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bradley\Documents\CougsInSpace\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC7AFFB-774E-4C3C-9AF6-70F2F1D6A1D5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB332791-2BBA-47AE-9A9B-E7563CD00DD0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="6" xr2:uid="{42A108CB-A0BE-49ED-8B7A-3FB1AB856735}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{42A108CB-A0BE-49ED-8B7A-3FB1AB856735}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3422" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3464" uniqueCount="594">
   <si>
     <t>Vendors have been selected by high reputability and lowest price</t>
   </si>
@@ -1694,6 +1694,129 @@
   </si>
   <si>
     <t>62-xxxx: All other ICs</t>
+  </si>
+  <si>
+    <t>63-0001</t>
+  </si>
+  <si>
+    <t>63-0002</t>
+  </si>
+  <si>
+    <t>63-0003</t>
+  </si>
+  <si>
+    <t>63-0004</t>
+  </si>
+  <si>
+    <t>Venus838FLPx-L</t>
+  </si>
+  <si>
+    <t>VENUS-1010</t>
+  </si>
+  <si>
+    <t>65-0001</t>
+  </si>
+  <si>
+    <t>Venus838FLPx-SPC</t>
+  </si>
+  <si>
+    <t>NavSpark</t>
+  </si>
+  <si>
+    <t>21-1003</t>
+  </si>
+  <si>
+    <t>21-1023</t>
+  </si>
+  <si>
+    <t>21-1002</t>
+  </si>
+  <si>
+    <t>21-1212</t>
+  </si>
+  <si>
+    <t>21-1500</t>
+  </si>
+  <si>
+    <t>21-1583</t>
+  </si>
+  <si>
+    <t>21-2003</t>
+  </si>
+  <si>
+    <t>21-2203</t>
+  </si>
+  <si>
+    <t>21-3163</t>
+  </si>
+  <si>
+    <t>21-3303</t>
+  </si>
+  <si>
+    <t>21-3603</t>
+  </si>
+  <si>
+    <t>21-1001</t>
+  </si>
+  <si>
+    <t>21-1004</t>
+  </si>
+  <si>
+    <t>21-2201</t>
+  </si>
+  <si>
+    <t>21-2204</t>
+  </si>
+  <si>
+    <t>21-6203</t>
+  </si>
+  <si>
+    <t>21-3301</t>
+  </si>
+  <si>
+    <t>21-3300</t>
+  </si>
+  <si>
+    <t>21-3302</t>
+  </si>
+  <si>
+    <t>21-3922</t>
+  </si>
+  <si>
+    <t>21-4702</t>
+  </si>
+  <si>
+    <t>21-0.05</t>
+  </si>
+  <si>
+    <t>21-5363</t>
+  </si>
+  <si>
+    <t>21-5600</t>
+  </si>
+  <si>
+    <t>21-8203</t>
+  </si>
+  <si>
+    <t>23-0.10</t>
+  </si>
+  <si>
+    <t>23-0.01</t>
+  </si>
+  <si>
+    <t>25-10.0</t>
+  </si>
+  <si>
+    <t>26-1002</t>
+  </si>
+  <si>
+    <t>26-2203</t>
+  </si>
+  <si>
+    <t>26-6802</t>
+  </si>
+  <si>
+    <t>26-3001</t>
   </si>
 </sst>
 </file>
@@ -1786,7 +1909,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1822,22 +1945,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2213,9 +2337,9 @@
   <dimension ref="A1:J164"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="10" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="A75" sqref="A75:B75"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,10 +2349,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="26"/>
       <c r="C1" s="1"/>
       <c r="D1" s="21"/>
       <c r="E1" s="1"/>
@@ -2237,10 +2361,10 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="2"/>
@@ -2250,18 +2374,18 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="7"/>
       <c r="E4" s="7"/>
     </row>
@@ -2369,732 +2493,777 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="29" t="s">
         <v>411</v>
       </c>
-      <c r="B24" s="24"/>
+      <c r="B24" s="29"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="29" t="s">
         <v>412</v>
       </c>
-      <c r="B25" s="24"/>
+      <c r="B25" s="29"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="29" t="s">
         <v>413</v>
       </c>
-      <c r="B26" s="24"/>
+      <c r="B26" s="29"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="29" t="s">
         <v>414</v>
       </c>
-      <c r="B27" s="24"/>
+      <c r="B27" s="29"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="29" t="s">
         <v>415</v>
       </c>
-      <c r="B28" s="24"/>
+      <c r="B28" s="29"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="29" t="s">
         <v>416</v>
       </c>
-      <c r="B29" s="24"/>
+      <c r="B29" s="29"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="29" t="s">
         <v>417</v>
       </c>
-      <c r="B30" s="24"/>
+      <c r="B30" s="29"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="29" t="s">
         <v>418</v>
       </c>
-      <c r="B31" s="24"/>
+      <c r="B31" s="29"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="29" t="s">
         <v>419</v>
       </c>
-      <c r="B32" s="24"/>
+      <c r="B32" s="29"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="29" t="s">
         <v>420</v>
       </c>
-      <c r="B33" s="24"/>
+      <c r="B33" s="29"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="30" t="s">
         <v>516</v>
       </c>
-      <c r="B34" s="25"/>
+      <c r="B34" s="30"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="29" t="s">
         <v>517</v>
       </c>
-      <c r="B35" s="24"/>
+      <c r="B35" s="29"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="29" t="s">
         <v>518</v>
       </c>
-      <c r="B36" s="24"/>
+      <c r="B36" s="29"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="29" t="s">
         <v>519</v>
       </c>
-      <c r="B37" s="24"/>
+      <c r="B37" s="29"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="30" t="s">
         <v>520</v>
       </c>
-      <c r="B38" s="25"/>
+      <c r="B38" s="30"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="30" t="s">
         <v>521</v>
       </c>
-      <c r="B39" s="25"/>
+      <c r="B39" s="30"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="30" t="s">
         <v>514</v>
       </c>
-      <c r="B40" s="25"/>
+      <c r="B40" s="30"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="30" t="s">
         <v>515</v>
       </c>
-      <c r="B41" s="25"/>
+      <c r="B41" s="30"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="30" t="s">
         <v>523</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="30"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="30" t="s">
         <v>527</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="30"/>
     </row>
     <row r="44" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="31" t="s">
         <v>471</v>
       </c>
-      <c r="B44" s="26"/>
+      <c r="B44" s="31"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="29" t="s">
         <v>462</v>
       </c>
-      <c r="B45" s="24"/>
+      <c r="B45" s="29"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="24" t="s">
+      <c r="A46" s="29" t="s">
         <v>463</v>
       </c>
-      <c r="B46" s="24"/>
+      <c r="B46" s="29"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="29" t="s">
         <v>464</v>
       </c>
-      <c r="B47" s="24"/>
+      <c r="B47" s="29"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="24" t="s">
+      <c r="A48" s="29" t="s">
         <v>465</v>
       </c>
-      <c r="B48" s="24"/>
+      <c r="B48" s="29"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="29" t="s">
         <v>466</v>
       </c>
-      <c r="B49" s="24"/>
+      <c r="B49" s="29"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="29" t="s">
         <v>467</v>
       </c>
-      <c r="B50" s="24"/>
+      <c r="B50" s="29"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="24" t="s">
+      <c r="A51" s="29" t="s">
         <v>468</v>
       </c>
-      <c r="B51" s="24"/>
+      <c r="B51" s="29"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="24" t="s">
+      <c r="A52" s="29" t="s">
         <v>469</v>
       </c>
-      <c r="B52" s="24"/>
+      <c r="B52" s="29"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="24" t="s">
+      <c r="A53" s="29" t="s">
         <v>470</v>
       </c>
-      <c r="B53" s="24"/>
+      <c r="B53" s="29"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="24" t="s">
+      <c r="A54" s="29" t="s">
         <v>451</v>
       </c>
-      <c r="B54" s="24"/>
+      <c r="B54" s="29"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="24" t="s">
+      <c r="A55" s="29" t="s">
         <v>452</v>
       </c>
-      <c r="B55" s="24"/>
+      <c r="B55" s="29"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="29" t="s">
         <v>453</v>
       </c>
-      <c r="B56" s="24"/>
+      <c r="B56" s="29"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="25" t="s">
+      <c r="A57" s="30" t="s">
         <v>454</v>
       </c>
-      <c r="B57" s="25"/>
+      <c r="B57" s="30"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="25" t="s">
+      <c r="A58" s="30" t="s">
         <v>455</v>
       </c>
-      <c r="B58" s="25"/>
+      <c r="B58" s="30"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="25" t="s">
+      <c r="A59" s="30" t="s">
         <v>456</v>
       </c>
-      <c r="B59" s="25"/>
+      <c r="B59" s="30"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="25" t="s">
+      <c r="A60" s="30" t="s">
         <v>457</v>
       </c>
-      <c r="B60" s="25"/>
+      <c r="B60" s="30"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="25" t="s">
+      <c r="A61" s="30" t="s">
         <v>458</v>
       </c>
-      <c r="B61" s="25"/>
+      <c r="B61" s="30"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="24" t="s">
+      <c r="A62" s="29" t="s">
         <v>510</v>
       </c>
-      <c r="B62" s="24"/>
+      <c r="B62" s="29"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="24" t="s">
+      <c r="A63" s="29" t="s">
         <v>511</v>
       </c>
-      <c r="B63" s="24"/>
+      <c r="B63" s="29"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="24" t="s">
+      <c r="A64" s="29" t="s">
         <v>488</v>
       </c>
-      <c r="B64" s="24"/>
+      <c r="B64" s="29"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="24" t="s">
+      <c r="A65" s="29" t="s">
         <v>489</v>
       </c>
-      <c r="B65" s="24"/>
+      <c r="B65" s="29"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="24" t="s">
+      <c r="A66" s="29" t="s">
         <v>490</v>
       </c>
-      <c r="B66" s="24"/>
+      <c r="B66" s="29"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="24" t="s">
+      <c r="A67" s="29" t="s">
         <v>491</v>
       </c>
-      <c r="B67" s="24"/>
+      <c r="B67" s="29"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="24" t="s">
+      <c r="A68" s="29" t="s">
         <v>492</v>
       </c>
-      <c r="B68" s="24"/>
+      <c r="B68" s="29"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="24" t="s">
+      <c r="A69" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="B69" s="24"/>
+      <c r="B69" s="29"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="24" t="s">
+      <c r="A70" s="29" t="s">
         <v>494</v>
       </c>
-      <c r="B70" s="24"/>
+      <c r="B70" s="29"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="24" t="s">
+      <c r="A71" s="29" t="s">
         <v>495</v>
       </c>
-      <c r="B71" s="24"/>
+      <c r="B71" s="29"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="24" t="s">
+      <c r="A72" s="29" t="s">
         <v>496</v>
       </c>
-      <c r="B72" s="24"/>
+      <c r="B72" s="29"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="24" t="s">
+      <c r="A73" s="29" t="s">
         <v>497</v>
       </c>
-      <c r="B73" s="24"/>
+      <c r="B73" s="29"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="25" t="s">
+      <c r="A74" s="30" t="s">
         <v>529</v>
       </c>
-      <c r="B74" s="25"/>
+      <c r="B74" s="30"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="25" t="s">
+      <c r="A75" s="30" t="s">
         <v>530</v>
       </c>
-      <c r="B75" s="25"/>
+      <c r="B75" s="30"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="25" t="s">
+      <c r="A76" s="30" t="s">
         <v>552</v>
       </c>
-      <c r="B76" s="25"/>
+      <c r="B76" s="30"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="25" t="s">
+      <c r="A77" s="30" t="s">
         <v>531</v>
       </c>
-      <c r="B77" s="25"/>
+      <c r="B77" s="30"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="25" t="s">
+      <c r="A78" s="30" t="s">
         <v>532</v>
       </c>
-      <c r="B78" s="25"/>
+      <c r="B78" s="30"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="25" t="s">
+      <c r="A79" s="30" t="s">
         <v>533</v>
       </c>
-      <c r="B79" s="25"/>
+      <c r="B79" s="30"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="25" t="s">
+      <c r="A80" s="30" t="s">
         <v>534</v>
       </c>
-      <c r="B80" s="25"/>
+      <c r="B80" s="30"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="25" t="s">
+      <c r="A81" s="30" t="s">
         <v>535</v>
       </c>
-      <c r="B81" s="25"/>
+      <c r="B81" s="30"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="24"/>
-      <c r="B82" s="24"/>
+      <c r="A82" s="29"/>
+      <c r="B82" s="29"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="24"/>
-      <c r="B83" s="24"/>
+      <c r="A83" s="29"/>
+      <c r="B83" s="29"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="24"/>
-      <c r="B84" s="24"/>
+      <c r="A84" s="29"/>
+      <c r="B84" s="29"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="24"/>
-      <c r="B85" s="24"/>
+      <c r="A85" s="29"/>
+      <c r="B85" s="29"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="24"/>
-      <c r="B86" s="24"/>
+      <c r="A86" s="29"/>
+      <c r="B86" s="29"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="24"/>
-      <c r="B87" s="24"/>
+      <c r="A87" s="29"/>
+      <c r="B87" s="29"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="24"/>
-      <c r="B88" s="24"/>
+      <c r="A88" s="29"/>
+      <c r="B88" s="29"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="24"/>
-      <c r="B89" s="24"/>
+      <c r="A89" s="29"/>
+      <c r="B89" s="29"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="24"/>
-      <c r="B90" s="24"/>
+      <c r="A90" s="29"/>
+      <c r="B90" s="29"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="24"/>
-      <c r="B91" s="24"/>
+      <c r="A91" s="29"/>
+      <c r="B91" s="29"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="24"/>
-      <c r="B92" s="24"/>
+      <c r="A92" s="29"/>
+      <c r="B92" s="29"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="24"/>
-      <c r="B93" s="24"/>
+      <c r="A93" s="29"/>
+      <c r="B93" s="29"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="24"/>
-      <c r="B94" s="24"/>
+      <c r="A94" s="29"/>
+      <c r="B94" s="29"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="24"/>
-      <c r="B95" s="24"/>
+      <c r="A95" s="29"/>
+      <c r="B95" s="29"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="24"/>
-      <c r="B96" s="24"/>
+      <c r="A96" s="29"/>
+      <c r="B96" s="29"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="24"/>
-      <c r="B97" s="24"/>
+      <c r="A97" s="29"/>
+      <c r="B97" s="29"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="24"/>
-      <c r="B98" s="24"/>
+      <c r="A98" s="29"/>
+      <c r="B98" s="29"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="24"/>
-      <c r="B99" s="24"/>
+      <c r="A99" s="29"/>
+      <c r="B99" s="29"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="24"/>
-      <c r="B100" s="24"/>
+      <c r="A100" s="29"/>
+      <c r="B100" s="29"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="24"/>
-      <c r="B101" s="24"/>
+      <c r="A101" s="29"/>
+      <c r="B101" s="29"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="24"/>
-      <c r="B102" s="24"/>
+      <c r="A102" s="29"/>
+      <c r="B102" s="29"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="24"/>
-      <c r="B103" s="24"/>
+      <c r="A103" s="29"/>
+      <c r="B103" s="29"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="24"/>
-      <c r="B104" s="24"/>
+      <c r="A104" s="29"/>
+      <c r="B104" s="29"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="24"/>
-      <c r="B105" s="24"/>
+      <c r="A105" s="29"/>
+      <c r="B105" s="29"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="24"/>
-      <c r="B106" s="24"/>
+      <c r="A106" s="29"/>
+      <c r="B106" s="29"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="24"/>
-      <c r="B107" s="24"/>
+      <c r="A107" s="29"/>
+      <c r="B107" s="29"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="24"/>
-      <c r="B108" s="24"/>
+      <c r="A108" s="29"/>
+      <c r="B108" s="29"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="24"/>
-      <c r="B109" s="24"/>
+      <c r="A109" s="29"/>
+      <c r="B109" s="29"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="24"/>
-      <c r="B110" s="24"/>
+      <c r="A110" s="29"/>
+      <c r="B110" s="29"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="24"/>
-      <c r="B111" s="24"/>
+      <c r="A111" s="29"/>
+      <c r="B111" s="29"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="24"/>
-      <c r="B112" s="24"/>
+      <c r="A112" s="29"/>
+      <c r="B112" s="29"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="24"/>
-      <c r="B113" s="24"/>
+      <c r="A113" s="29"/>
+      <c r="B113" s="29"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="24"/>
-      <c r="B114" s="24"/>
+      <c r="A114" s="29"/>
+      <c r="B114" s="29"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="24"/>
-      <c r="B115" s="24"/>
+      <c r="A115" s="29"/>
+      <c r="B115" s="29"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="24"/>
-      <c r="B116" s="24"/>
+      <c r="A116" s="29"/>
+      <c r="B116" s="29"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="24"/>
-      <c r="B117" s="24"/>
+      <c r="A117" s="29"/>
+      <c r="B117" s="29"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="24"/>
-      <c r="B118" s="24"/>
+      <c r="A118" s="29"/>
+      <c r="B118" s="29"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="24"/>
-      <c r="B119" s="24"/>
+      <c r="A119" s="29"/>
+      <c r="B119" s="29"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="24"/>
-      <c r="B120" s="24"/>
+      <c r="A120" s="29"/>
+      <c r="B120" s="29"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="24"/>
-      <c r="B121" s="24"/>
+      <c r="A121" s="29"/>
+      <c r="B121" s="29"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="24"/>
-      <c r="B122" s="24"/>
+      <c r="A122" s="29"/>
+      <c r="B122" s="29"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="24"/>
-      <c r="B123" s="24"/>
+      <c r="A123" s="29"/>
+      <c r="B123" s="29"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="24"/>
-      <c r="B124" s="24"/>
+      <c r="A124" s="29"/>
+      <c r="B124" s="29"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="24"/>
-      <c r="B125" s="24"/>
+      <c r="A125" s="29"/>
+      <c r="B125" s="29"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="24"/>
-      <c r="B126" s="24"/>
+      <c r="A126" s="29"/>
+      <c r="B126" s="29"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="24"/>
-      <c r="B127" s="24"/>
+      <c r="A127" s="29"/>
+      <c r="B127" s="29"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="24"/>
-      <c r="B128" s="24"/>
+      <c r="A128" s="29"/>
+      <c r="B128" s="29"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="24"/>
-      <c r="B129" s="24"/>
+      <c r="A129" s="29"/>
+      <c r="B129" s="29"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="24"/>
-      <c r="B130" s="24"/>
+      <c r="A130" s="29"/>
+      <c r="B130" s="29"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="24"/>
-      <c r="B131" s="24"/>
+      <c r="A131" s="29"/>
+      <c r="B131" s="29"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="24"/>
-      <c r="B132" s="24"/>
+      <c r="A132" s="29"/>
+      <c r="B132" s="29"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="24"/>
-      <c r="B133" s="24"/>
+      <c r="A133" s="29"/>
+      <c r="B133" s="29"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="24"/>
-      <c r="B134" s="24"/>
+      <c r="A134" s="29"/>
+      <c r="B134" s="29"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="24"/>
-      <c r="B135" s="24"/>
+      <c r="A135" s="29"/>
+      <c r="B135" s="29"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="24"/>
-      <c r="B136" s="24"/>
+      <c r="A136" s="29"/>
+      <c r="B136" s="29"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="24"/>
-      <c r="B137" s="24"/>
+      <c r="A137" s="29"/>
+      <c r="B137" s="29"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="24"/>
-      <c r="B138" s="24"/>
+      <c r="A138" s="29"/>
+      <c r="B138" s="29"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="24"/>
-      <c r="B139" s="24"/>
+      <c r="A139" s="29"/>
+      <c r="B139" s="29"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="24"/>
-      <c r="B140" s="24"/>
+      <c r="A140" s="29"/>
+      <c r="B140" s="29"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="24"/>
-      <c r="B141" s="24"/>
+      <c r="A141" s="29"/>
+      <c r="B141" s="29"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="24"/>
-      <c r="B142" s="24"/>
+      <c r="A142" s="29"/>
+      <c r="B142" s="29"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="24"/>
-      <c r="B143" s="24"/>
+      <c r="A143" s="29"/>
+      <c r="B143" s="29"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="24"/>
-      <c r="B144" s="24"/>
+      <c r="A144" s="29"/>
+      <c r="B144" s="29"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="24"/>
-      <c r="B145" s="24"/>
+      <c r="A145" s="29"/>
+      <c r="B145" s="29"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="24"/>
-      <c r="B146" s="24"/>
+      <c r="A146" s="29"/>
+      <c r="B146" s="29"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="24"/>
-      <c r="B147" s="24"/>
+      <c r="A147" s="29"/>
+      <c r="B147" s="29"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="24"/>
-      <c r="B148" s="24"/>
+      <c r="A148" s="29"/>
+      <c r="B148" s="29"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="24"/>
-      <c r="B149" s="24"/>
+      <c r="A149" s="29"/>
+      <c r="B149" s="29"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="24"/>
-      <c r="B150" s="24"/>
+      <c r="A150" s="29"/>
+      <c r="B150" s="29"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="24"/>
-      <c r="B151" s="24"/>
+      <c r="A151" s="29"/>
+      <c r="B151" s="29"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="24"/>
-      <c r="B152" s="24"/>
+      <c r="A152" s="29"/>
+      <c r="B152" s="29"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="24"/>
-      <c r="B153" s="24"/>
+      <c r="A153" s="29"/>
+      <c r="B153" s="29"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="24"/>
-      <c r="B154" s="24"/>
+      <c r="A154" s="29"/>
+      <c r="B154" s="29"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="24"/>
-      <c r="B155" s="24"/>
+      <c r="A155" s="29"/>
+      <c r="B155" s="29"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="24"/>
-      <c r="B156" s="24"/>
+      <c r="A156" s="29"/>
+      <c r="B156" s="29"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="24"/>
-      <c r="B157" s="24"/>
+      <c r="A157" s="29"/>
+      <c r="B157" s="29"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="24"/>
-      <c r="B158" s="24"/>
+      <c r="A158" s="29"/>
+      <c r="B158" s="29"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="24"/>
-      <c r="B159" s="24"/>
+      <c r="A159" s="29"/>
+      <c r="B159" s="29"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="24"/>
-      <c r="B160" s="24"/>
+      <c r="A160" s="29"/>
+      <c r="B160" s="29"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="24"/>
-      <c r="B161" s="24"/>
+      <c r="A161" s="29"/>
+      <c r="B161" s="29"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="24"/>
-      <c r="B162" s="24"/>
+      <c r="A162" s="29"/>
+      <c r="B162" s="29"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="24"/>
-      <c r="B163" s="24"/>
+      <c r="A163" s="29"/>
+      <c r="B163" s="29"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="24"/>
-      <c r="B164" s="24"/>
+      <c r="A164" s="29"/>
+      <c r="B164" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="145">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A161:B161"/>
+    <mergeCell ref="A162:B162"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="A164:B164"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="A157:B157"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="A72:B72"/>
@@ -3105,96 +3274,51 @@
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A68:B68"/>
     <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="A161:B161"/>
-    <mergeCell ref="A162:B162"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="A164:B164"/>
-    <mergeCell ref="A155:B155"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="A157:B157"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3206,8 +3330,8 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3224,17 +3348,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
@@ -8755,10 +8879,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD668FA6-C86B-4B15-9051-DF984B595504}">
-  <dimension ref="A1:H301"/>
+  <dimension ref="A1:I301"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8768,25 +8892,27 @@
     <col min="3" max="3" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="10"/>
+    <col min="6" max="6" width="17.7109375" style="24" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>108</v>
       </c>
@@ -8803,16 +8929,19 @@
         <v>4</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>4</v>
       </c>
@@ -8828,17 +8957,20 @@
       <c r="E4" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>23</v>
       </c>
@@ -8854,17 +8986,20 @@
       <c r="E5" s="5">
         <v>1608</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>8</v>
       </c>
@@ -8880,17 +9015,20 @@
       <c r="E6" s="5">
         <v>3216</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="5" t="s">
+        <v>587</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="I6" s="10" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>4</v>
       </c>
@@ -8906,17 +9044,20 @@
       <c r="E7" s="5">
         <v>1608</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="I7" s="10" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>12</v>
       </c>
@@ -8932,17 +9073,20 @@
       <c r="E8" s="5">
         <v>1608</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="I8" s="10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>10</v>
       </c>
@@ -8958,17 +9102,20 @@
       <c r="E9" s="5">
         <v>1632</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>363</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="I9" s="10" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>11</v>
       </c>
@@ -8984,17 +9131,20 @@
       <c r="E10" s="5">
         <v>3216</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="I10" s="10" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>5</v>
       </c>
@@ -9010,17 +9160,20 @@
       <c r="E11" s="5">
         <v>1608</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="I11" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>8</v>
       </c>
@@ -9036,17 +9189,20 @@
       <c r="E12" s="5">
         <v>1608</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="I12" s="10" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>4</v>
       </c>
@@ -9062,17 +9218,20 @@
       <c r="E13" s="5">
         <v>1608</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="I13" s="10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>42</v>
       </c>
@@ -9088,17 +9247,20 @@
       <c r="E14" s="5">
         <v>1608</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="H14" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="I14" s="10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>9</v>
       </c>
@@ -9114,17 +9276,20 @@
       <c r="E15" s="5">
         <v>1608</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="H15" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="I15" s="10" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>9</v>
       </c>
@@ -9140,17 +9305,20 @@
       <c r="E16" s="5">
         <v>1608</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="H16" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="I16" s="10" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -9166,17 +9334,20 @@
       <c r="E17" s="5">
         <v>1608</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="H17" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="I17" s="10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>4</v>
       </c>
@@ -9192,17 +9363,20 @@
       <c r="E18" s="5">
         <v>1608</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="5" t="s">
+        <v>568</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="H18" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="I18" s="10" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>6</v>
       </c>
@@ -9218,17 +9392,20 @@
       <c r="E19" s="5">
         <v>1608</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="G19" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="H19" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="I19" s="10" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>10</v>
       </c>
@@ -9244,17 +9421,20 @@
       <c r="E20" s="5">
         <v>1632</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="G20" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="H20" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="I20" s="10" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>4</v>
       </c>
@@ -9270,17 +9450,20 @@
       <c r="E21" s="5">
         <v>1608</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="H21" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="I21" s="10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>3</v>
       </c>
@@ -9296,17 +9479,20 @@
       <c r="E22" s="5">
         <v>1608</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="H22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="I22" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>9</v>
       </c>
@@ -9322,17 +9508,20 @@
       <c r="E23" s="5">
         <v>1608</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="G23" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="H23" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="I23" s="10" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>9</v>
       </c>
@@ -9348,17 +9537,20 @@
       <c r="E24" s="5">
         <v>1608</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="H24" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="I24" s="10" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>10</v>
       </c>
@@ -9374,17 +9566,20 @@
       <c r="E25" s="5">
         <v>1608</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="G25" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="H25" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="I25" s="10" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>8</v>
       </c>
@@ -9400,17 +9595,20 @@
       <c r="E26" s="5">
         <v>1608</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="G26" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="H26" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="I26" s="10" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>4</v>
       </c>
@@ -9426,17 +9624,20 @@
       <c r="E27" s="5">
         <v>1608</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="G27" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="H27" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="I27" s="10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>3</v>
       </c>
@@ -9452,17 +9653,20 @@
       <c r="E28" s="5">
         <v>1608</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="H28" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H28" s="10" t="s">
+      <c r="I28" s="10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>22</v>
       </c>
@@ -9478,17 +9682,20 @@
       <c r="E29" s="5">
         <v>1608</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="G29" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="H29" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="I29" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>8</v>
       </c>
@@ -9504,17 +9711,20 @@
       <c r="E30" s="5">
         <v>1608</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="G30" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="H30" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H30" s="10" t="s">
+      <c r="I30" s="10" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>74</v>
       </c>
@@ -9530,17 +9740,20 @@
       <c r="E31" s="5">
         <v>1608</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="G31" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="H31" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="I31" s="10" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>9</v>
       </c>
@@ -9556,17 +9769,20 @@
       <c r="E32" s="5">
         <v>1608</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="G32" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="H32" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="I32" s="10" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>5</v>
       </c>
@@ -9582,17 +9798,20 @@
       <c r="E33" s="5">
         <v>1608</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="G33" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="H33" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="I33" s="10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>25</v>
       </c>
@@ -9608,17 +9827,20 @@
       <c r="E34" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="5" t="s">
+        <v>593</v>
+      </c>
+      <c r="G34" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="H34" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H34" s="10" t="s">
+      <c r="I34" s="10" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>21</v>
       </c>
@@ -9635,76 +9857,79 @@
         <v>1608</v>
       </c>
       <c r="F35" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="H35" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H35" s="10" t="s">
+      <c r="I35" s="10" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C38" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C39" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C40" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C41" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C42" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C43" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C44" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C45" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C46" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C47" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
         <v>238</v>
       </c>
@@ -10975,12 +11200,12 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:H45">
+  <sortState ref="A4:I45">
     <sortCondition ref="D4:D45"/>
     <sortCondition ref="E4:E45"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C301">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
@@ -10996,7 +11221,7 @@
   <dimension ref="A1:I300"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11014,17 +11239,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -12696,17 +12921,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -14432,7 +14657,7 @@
   <dimension ref="A1:I299"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14450,17 +14675,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
@@ -14686,6 +14911,9 @@
       <c r="E10" s="10" t="s">
         <v>166</v>
       </c>
+      <c r="F10" s="22" t="s">
+        <v>553</v>
+      </c>
       <c r="G10" s="10" t="s">
         <v>256</v>
       </c>
@@ -14712,7 +14940,9 @@
       <c r="E11" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>554</v>
+      </c>
       <c r="G11" s="10" t="s">
         <v>176</v>
       </c>
@@ -14739,7 +14969,9 @@
       <c r="E12" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>555</v>
+      </c>
       <c r="G12" s="10" t="s">
         <v>260</v>
       </c>
@@ -14765,6 +14997,9 @@
       </c>
       <c r="E13" s="10" t="s">
         <v>166</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>556</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>263</v>
@@ -16272,8 +16507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D526D2F0-6B58-44A3-8176-A7A0AAEF1CB8}">
   <dimension ref="A1:I300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16285,23 +16520,23 @@
     <col min="5" max="5" width="16.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" style="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -16348,7 +16583,7 @@
       <c r="E4" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="25" t="s">
         <v>537</v>
       </c>
       <c r="G4" s="10" t="s">
@@ -16406,7 +16641,7 @@
       <c r="E6" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="25" t="s">
         <v>541</v>
       </c>
       <c r="G6" s="10" t="s">
@@ -16435,7 +16670,7 @@
       <c r="E7" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="25" t="s">
         <v>542</v>
       </c>
       <c r="G7" s="10" t="s">
@@ -16493,7 +16728,7 @@
       <c r="E9" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="25" t="s">
         <v>543</v>
       </c>
       <c r="G9" s="10" t="s">
@@ -16551,7 +16786,7 @@
       <c r="E11" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="25" t="s">
         <v>538</v>
       </c>
       <c r="G11" s="10" t="s">
@@ -16580,7 +16815,7 @@
       <c r="E12" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="25" t="s">
         <v>539</v>
       </c>
       <c r="G12" s="5" t="s">
@@ -16609,7 +16844,7 @@
       <c r="E13" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="25" t="s">
         <v>544</v>
       </c>
       <c r="G13" s="5" t="s">
@@ -16638,7 +16873,7 @@
       <c r="E14" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="25" t="s">
         <v>545</v>
       </c>
       <c r="G14" s="10" t="s">
@@ -16696,7 +16931,7 @@
       <c r="E16" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="25" t="s">
         <v>546</v>
       </c>
       <c r="G16" s="5" t="s">
@@ -16725,7 +16960,7 @@
       <c r="E17" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="25" t="s">
         <v>547</v>
       </c>
       <c r="G17" s="10" t="s">
@@ -16783,7 +17018,7 @@
       <c r="E19" s="10" t="s">
         <v>382</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="25" t="s">
         <v>548</v>
       </c>
       <c r="G19" s="10" t="s">
@@ -16812,7 +17047,7 @@
       <c r="E20" s="10" t="s">
         <v>386</v>
       </c>
-      <c r="F20" s="32" t="s">
+      <c r="F20" s="25" t="s">
         <v>549</v>
       </c>
       <c r="G20" s="10" t="s">
@@ -16841,7 +17076,7 @@
       <c r="E21" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="25" t="s">
         <v>550</v>
       </c>
       <c r="G21" s="10" t="s">
@@ -16870,7 +17105,7 @@
       <c r="E22" s="10" t="s">
         <v>398</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="25" t="s">
         <v>551</v>
       </c>
       <c r="G22" s="10" t="s">
@@ -16913,8 +17148,32 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="2" t="s">
-        <v>238</v>
+      <c r="A24" s="10">
+        <v>0</v>
+      </c>
+      <c r="B24" s="10">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>557</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>560</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>561</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -18334,17 +18593,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -20041,20 +20300,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
       <c r="D1" s="17"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="18" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Added CougSat Bus Socket
</commit_message>
<xml_diff>
--- a/CougsInSpace-Inventory.xlsx
+++ b/CougsInSpace-Inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bradley\Documents\CougsInSpace\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB332791-2BBA-47AE-9A9B-E7563CD00DD0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA72589-B5B8-4CFA-A148-4B90BAA4149A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{42A108CB-A0BE-49ED-8B7A-3FB1AB856735}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="4" xr2:uid="{42A108CB-A0BE-49ED-8B7A-3FB1AB856735}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3464" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3470" uniqueCount="599">
   <si>
     <t>Vendors have been selected by high reputability and lowest price</t>
   </si>
@@ -1817,6 +1817,21 @@
   </si>
   <si>
     <t>26-3001</t>
+  </si>
+  <si>
+    <t>04-0006</t>
+  </si>
+  <si>
+    <t>CougSat Socket</t>
+  </si>
+  <si>
+    <t>SODIMM_DDR1</t>
+  </si>
+  <si>
+    <t>2040910-1</t>
+  </si>
+  <si>
+    <t>A118337-ND</t>
   </si>
 </sst>
 </file>
@@ -1909,7 +1924,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1946,16 +1961,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2337,7 +2353,7 @@
   <dimension ref="A1:J164"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="10" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="bottomLeft" activeCell="A34" sqref="A34:B34"/>
     </sheetView>
@@ -2349,10 +2365,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="30"/>
       <c r="C1" s="1"/>
       <c r="D1" s="21"/>
       <c r="E1" s="1"/>
@@ -2361,10 +2377,10 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="2"/>
@@ -2374,18 +2390,18 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="7"/>
       <c r="E4" s="7"/>
     </row>
@@ -2493,687 +2509,822 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="27" t="s">
         <v>411</v>
       </c>
-      <c r="B24" s="29"/>
+      <c r="B24" s="27"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="27" t="s">
         <v>412</v>
       </c>
-      <c r="B25" s="29"/>
+      <c r="B25" s="27"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="27" t="s">
         <v>413</v>
       </c>
-      <c r="B26" s="29"/>
+      <c r="B26" s="27"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="27" t="s">
         <v>414</v>
       </c>
-      <c r="B27" s="29"/>
+      <c r="B27" s="27"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="27" t="s">
         <v>415</v>
       </c>
-      <c r="B28" s="29"/>
+      <c r="B28" s="27"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="27" t="s">
         <v>416</v>
       </c>
-      <c r="B29" s="29"/>
+      <c r="B29" s="27"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="27" t="s">
         <v>417</v>
       </c>
-      <c r="B30" s="29"/>
+      <c r="B30" s="27"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="27" t="s">
         <v>418</v>
       </c>
-      <c r="B31" s="29"/>
+      <c r="B31" s="27"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="27" t="s">
         <v>419</v>
       </c>
-      <c r="B32" s="29"/>
+      <c r="B32" s="27"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="27" t="s">
         <v>420</v>
       </c>
-      <c r="B33" s="29"/>
+      <c r="B33" s="27"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="28" t="s">
         <v>516</v>
       </c>
-      <c r="B34" s="30"/>
+      <c r="B34" s="28"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="27" t="s">
         <v>517</v>
       </c>
-      <c r="B35" s="29"/>
+      <c r="B35" s="27"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="27" t="s">
         <v>518</v>
       </c>
-      <c r="B36" s="29"/>
+      <c r="B36" s="27"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="27" t="s">
         <v>519</v>
       </c>
-      <c r="B37" s="29"/>
+      <c r="B37" s="27"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="28" t="s">
         <v>520</v>
       </c>
-      <c r="B38" s="30"/>
+      <c r="B38" s="28"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="28" t="s">
         <v>521</v>
       </c>
-      <c r="B39" s="30"/>
+      <c r="B39" s="28"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="28" t="s">
         <v>514</v>
       </c>
-      <c r="B40" s="30"/>
+      <c r="B40" s="28"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="28" t="s">
         <v>515</v>
       </c>
-      <c r="B41" s="30"/>
+      <c r="B41" s="28"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="28" t="s">
         <v>523</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="28"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="28" t="s">
         <v>527</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="29" t="s">
         <v>471</v>
       </c>
-      <c r="B44" s="31"/>
+      <c r="B44" s="29"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="27" t="s">
         <v>462</v>
       </c>
-      <c r="B45" s="29"/>
+      <c r="B45" s="27"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="27" t="s">
         <v>463</v>
       </c>
-      <c r="B46" s="29"/>
+      <c r="B46" s="27"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="27" t="s">
         <v>464</v>
       </c>
-      <c r="B47" s="29"/>
+      <c r="B47" s="27"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="27" t="s">
         <v>465</v>
       </c>
-      <c r="B48" s="29"/>
+      <c r="B48" s="27"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="27" t="s">
         <v>466</v>
       </c>
-      <c r="B49" s="29"/>
+      <c r="B49" s="27"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="27" t="s">
         <v>467</v>
       </c>
-      <c r="B50" s="29"/>
+      <c r="B50" s="27"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="29" t="s">
+      <c r="A51" s="27" t="s">
         <v>468</v>
       </c>
-      <c r="B51" s="29"/>
+      <c r="B51" s="27"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="29" t="s">
+      <c r="A52" s="27" t="s">
         <v>469</v>
       </c>
-      <c r="B52" s="29"/>
+      <c r="B52" s="27"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="27" t="s">
         <v>470</v>
       </c>
-      <c r="B53" s="29"/>
+      <c r="B53" s="27"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="29" t="s">
+      <c r="A54" s="27" t="s">
         <v>451</v>
       </c>
-      <c r="B54" s="29"/>
+      <c r="B54" s="27"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="29" t="s">
+      <c r="A55" s="27" t="s">
         <v>452</v>
       </c>
-      <c r="B55" s="29"/>
+      <c r="B55" s="27"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="27" t="s">
         <v>453</v>
       </c>
-      <c r="B56" s="29"/>
+      <c r="B56" s="27"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="30" t="s">
+      <c r="A57" s="28" t="s">
         <v>454</v>
       </c>
-      <c r="B57" s="30"/>
+      <c r="B57" s="28"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="30" t="s">
+      <c r="A58" s="28" t="s">
         <v>455</v>
       </c>
-      <c r="B58" s="30"/>
+      <c r="B58" s="28"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="30" t="s">
+      <c r="A59" s="28" t="s">
         <v>456</v>
       </c>
-      <c r="B59" s="30"/>
+      <c r="B59" s="28"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="30" t="s">
+      <c r="A60" s="28" t="s">
         <v>457</v>
       </c>
-      <c r="B60" s="30"/>
+      <c r="B60" s="28"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="30" t="s">
+      <c r="A61" s="28" t="s">
         <v>458</v>
       </c>
-      <c r="B61" s="30"/>
+      <c r="B61" s="28"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="29" t="s">
+      <c r="A62" s="27" t="s">
         <v>510</v>
       </c>
-      <c r="B62" s="29"/>
+      <c r="B62" s="27"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="29" t="s">
+      <c r="A63" s="27" t="s">
         <v>511</v>
       </c>
-      <c r="B63" s="29"/>
+      <c r="B63" s="27"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="29" t="s">
+      <c r="A64" s="27" t="s">
         <v>488</v>
       </c>
-      <c r="B64" s="29"/>
+      <c r="B64" s="27"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="29" t="s">
+      <c r="A65" s="27" t="s">
         <v>489</v>
       </c>
-      <c r="B65" s="29"/>
+      <c r="B65" s="27"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="29" t="s">
+      <c r="A66" s="27" t="s">
         <v>490</v>
       </c>
-      <c r="B66" s="29"/>
+      <c r="B66" s="27"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="29" t="s">
+      <c r="A67" s="27" t="s">
         <v>491</v>
       </c>
-      <c r="B67" s="29"/>
+      <c r="B67" s="27"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="29" t="s">
+      <c r="A68" s="27" t="s">
         <v>492</v>
       </c>
-      <c r="B68" s="29"/>
+      <c r="B68" s="27"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="29" t="s">
+      <c r="A69" s="27" t="s">
         <v>493</v>
       </c>
-      <c r="B69" s="29"/>
+      <c r="B69" s="27"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="29" t="s">
+      <c r="A70" s="27" t="s">
         <v>494</v>
       </c>
-      <c r="B70" s="29"/>
+      <c r="B70" s="27"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="29" t="s">
+      <c r="A71" s="27" t="s">
         <v>495</v>
       </c>
-      <c r="B71" s="29"/>
+      <c r="B71" s="27"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="29" t="s">
+      <c r="A72" s="27" t="s">
         <v>496</v>
       </c>
-      <c r="B72" s="29"/>
+      <c r="B72" s="27"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="29" t="s">
+      <c r="A73" s="27" t="s">
         <v>497</v>
       </c>
-      <c r="B73" s="29"/>
+      <c r="B73" s="27"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="30" t="s">
+      <c r="A74" s="28" t="s">
         <v>529</v>
       </c>
-      <c r="B74" s="30"/>
+      <c r="B74" s="28"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="30" t="s">
+      <c r="A75" s="28" t="s">
         <v>530</v>
       </c>
-      <c r="B75" s="30"/>
+      <c r="B75" s="28"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="30" t="s">
+      <c r="A76" s="28" t="s">
         <v>552</v>
       </c>
-      <c r="B76" s="30"/>
+      <c r="B76" s="28"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="30" t="s">
+      <c r="A77" s="28" t="s">
         <v>531</v>
       </c>
-      <c r="B77" s="30"/>
+      <c r="B77" s="28"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="30" t="s">
+      <c r="A78" s="28" t="s">
         <v>532</v>
       </c>
-      <c r="B78" s="30"/>
+      <c r="B78" s="28"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="30" t="s">
+      <c r="A79" s="28" t="s">
         <v>533</v>
       </c>
-      <c r="B79" s="30"/>
+      <c r="B79" s="28"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="30" t="s">
+      <c r="A80" s="28" t="s">
         <v>534</v>
       </c>
-      <c r="B80" s="30"/>
+      <c r="B80" s="28"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="30" t="s">
+      <c r="A81" s="28" t="s">
         <v>535</v>
       </c>
-      <c r="B81" s="30"/>
+      <c r="B81" s="28"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="29"/>
-      <c r="B82" s="29"/>
+      <c r="A82" s="27"/>
+      <c r="B82" s="27"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="29"/>
-      <c r="B83" s="29"/>
+      <c r="A83" s="27"/>
+      <c r="B83" s="27"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="29"/>
-      <c r="B84" s="29"/>
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="29"/>
-      <c r="B85" s="29"/>
+      <c r="A85" s="27"/>
+      <c r="B85" s="27"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="29"/>
-      <c r="B86" s="29"/>
+      <c r="A86" s="27"/>
+      <c r="B86" s="27"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="29"/>
-      <c r="B87" s="29"/>
+      <c r="A87" s="27"/>
+      <c r="B87" s="27"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="29"/>
-      <c r="B88" s="29"/>
+      <c r="A88" s="27"/>
+      <c r="B88" s="27"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="29"/>
-      <c r="B89" s="29"/>
+      <c r="A89" s="27"/>
+      <c r="B89" s="27"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="29"/>
-      <c r="B90" s="29"/>
+      <c r="A90" s="27"/>
+      <c r="B90" s="27"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="29"/>
-      <c r="B91" s="29"/>
+      <c r="A91" s="27"/>
+      <c r="B91" s="27"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="29"/>
-      <c r="B92" s="29"/>
+      <c r="A92" s="27"/>
+      <c r="B92" s="27"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="29"/>
-      <c r="B93" s="29"/>
+      <c r="A93" s="27"/>
+      <c r="B93" s="27"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="29"/>
-      <c r="B94" s="29"/>
+      <c r="A94" s="27"/>
+      <c r="B94" s="27"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="29"/>
-      <c r="B95" s="29"/>
+      <c r="A95" s="27"/>
+      <c r="B95" s="27"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="29"/>
-      <c r="B96" s="29"/>
+      <c r="A96" s="27"/>
+      <c r="B96" s="27"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="29"/>
-      <c r="B97" s="29"/>
+      <c r="A97" s="27"/>
+      <c r="B97" s="27"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="29"/>
-      <c r="B98" s="29"/>
+      <c r="A98" s="27"/>
+      <c r="B98" s="27"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="29"/>
-      <c r="B99" s="29"/>
+      <c r="A99" s="27"/>
+      <c r="B99" s="27"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="29"/>
-      <c r="B100" s="29"/>
+      <c r="A100" s="27"/>
+      <c r="B100" s="27"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="29"/>
-      <c r="B101" s="29"/>
+      <c r="A101" s="27"/>
+      <c r="B101" s="27"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="29"/>
-      <c r="B102" s="29"/>
+      <c r="A102" s="27"/>
+      <c r="B102" s="27"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="29"/>
-      <c r="B103" s="29"/>
+      <c r="A103" s="27"/>
+      <c r="B103" s="27"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="29"/>
-      <c r="B104" s="29"/>
+      <c r="A104" s="27"/>
+      <c r="B104" s="27"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="29"/>
-      <c r="B105" s="29"/>
+      <c r="A105" s="27"/>
+      <c r="B105" s="27"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="29"/>
-      <c r="B106" s="29"/>
+      <c r="A106" s="27"/>
+      <c r="B106" s="27"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="29"/>
-      <c r="B107" s="29"/>
+      <c r="A107" s="27"/>
+      <c r="B107" s="27"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="29"/>
-      <c r="B108" s="29"/>
+      <c r="A108" s="27"/>
+      <c r="B108" s="27"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="29"/>
-      <c r="B109" s="29"/>
+      <c r="A109" s="27"/>
+      <c r="B109" s="27"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="29"/>
-      <c r="B110" s="29"/>
+      <c r="A110" s="27"/>
+      <c r="B110" s="27"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="29"/>
-      <c r="B111" s="29"/>
+      <c r="A111" s="27"/>
+      <c r="B111" s="27"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="29"/>
-      <c r="B112" s="29"/>
+      <c r="A112" s="27"/>
+      <c r="B112" s="27"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="29"/>
-      <c r="B113" s="29"/>
+      <c r="A113" s="27"/>
+      <c r="B113" s="27"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="29"/>
-      <c r="B114" s="29"/>
+      <c r="A114" s="27"/>
+      <c r="B114" s="27"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="29"/>
-      <c r="B115" s="29"/>
+      <c r="A115" s="27"/>
+      <c r="B115" s="27"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="29"/>
-      <c r="B116" s="29"/>
+      <c r="A116" s="27"/>
+      <c r="B116" s="27"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="29"/>
-      <c r="B117" s="29"/>
+      <c r="A117" s="27"/>
+      <c r="B117" s="27"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="29"/>
-      <c r="B118" s="29"/>
+      <c r="A118" s="27"/>
+      <c r="B118" s="27"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="29"/>
-      <c r="B119" s="29"/>
+      <c r="A119" s="27"/>
+      <c r="B119" s="27"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="29"/>
-      <c r="B120" s="29"/>
+      <c r="A120" s="27"/>
+      <c r="B120" s="27"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="29"/>
-      <c r="B121" s="29"/>
+      <c r="A121" s="27"/>
+      <c r="B121" s="27"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="29"/>
-      <c r="B122" s="29"/>
+      <c r="A122" s="27"/>
+      <c r="B122" s="27"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="29"/>
-      <c r="B123" s="29"/>
+      <c r="A123" s="27"/>
+      <c r="B123" s="27"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="29"/>
-      <c r="B124" s="29"/>
+      <c r="A124" s="27"/>
+      <c r="B124" s="27"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="29"/>
-      <c r="B125" s="29"/>
+      <c r="A125" s="27"/>
+      <c r="B125" s="27"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="29"/>
-      <c r="B126" s="29"/>
+      <c r="A126" s="27"/>
+      <c r="B126" s="27"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="29"/>
-      <c r="B127" s="29"/>
+      <c r="A127" s="27"/>
+      <c r="B127" s="27"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="29"/>
-      <c r="B128" s="29"/>
+      <c r="A128" s="27"/>
+      <c r="B128" s="27"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="29"/>
-      <c r="B129" s="29"/>
+      <c r="A129" s="27"/>
+      <c r="B129" s="27"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="29"/>
-      <c r="B130" s="29"/>
+      <c r="A130" s="27"/>
+      <c r="B130" s="27"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="29"/>
-      <c r="B131" s="29"/>
+      <c r="A131" s="27"/>
+      <c r="B131" s="27"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="29"/>
-      <c r="B132" s="29"/>
+      <c r="A132" s="27"/>
+      <c r="B132" s="27"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="29"/>
-      <c r="B133" s="29"/>
+      <c r="A133" s="27"/>
+      <c r="B133" s="27"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="29"/>
-      <c r="B134" s="29"/>
+      <c r="A134" s="27"/>
+      <c r="B134" s="27"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="29"/>
-      <c r="B135" s="29"/>
+      <c r="A135" s="27"/>
+      <c r="B135" s="27"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="29"/>
-      <c r="B136" s="29"/>
+      <c r="A136" s="27"/>
+      <c r="B136" s="27"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="29"/>
-      <c r="B137" s="29"/>
+      <c r="A137" s="27"/>
+      <c r="B137" s="27"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="29"/>
-      <c r="B138" s="29"/>
+      <c r="A138" s="27"/>
+      <c r="B138" s="27"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="29"/>
-      <c r="B139" s="29"/>
+      <c r="A139" s="27"/>
+      <c r="B139" s="27"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="29"/>
-      <c r="B140" s="29"/>
+      <c r="A140" s="27"/>
+      <c r="B140" s="27"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="29"/>
-      <c r="B141" s="29"/>
+      <c r="A141" s="27"/>
+      <c r="B141" s="27"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="29"/>
-      <c r="B142" s="29"/>
+      <c r="A142" s="27"/>
+      <c r="B142" s="27"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="29"/>
-      <c r="B143" s="29"/>
+      <c r="A143" s="27"/>
+      <c r="B143" s="27"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="29"/>
-      <c r="B144" s="29"/>
+      <c r="A144" s="27"/>
+      <c r="B144" s="27"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="29"/>
-      <c r="B145" s="29"/>
+      <c r="A145" s="27"/>
+      <c r="B145" s="27"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="29"/>
-      <c r="B146" s="29"/>
+      <c r="A146" s="27"/>
+      <c r="B146" s="27"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="29"/>
-      <c r="B147" s="29"/>
+      <c r="A147" s="27"/>
+      <c r="B147" s="27"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="29"/>
-      <c r="B148" s="29"/>
+      <c r="A148" s="27"/>
+      <c r="B148" s="27"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="29"/>
-      <c r="B149" s="29"/>
+      <c r="A149" s="27"/>
+      <c r="B149" s="27"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="29"/>
-      <c r="B150" s="29"/>
+      <c r="A150" s="27"/>
+      <c r="B150" s="27"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="29"/>
-      <c r="B151" s="29"/>
+      <c r="A151" s="27"/>
+      <c r="B151" s="27"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="29"/>
-      <c r="B152" s="29"/>
+      <c r="A152" s="27"/>
+      <c r="B152" s="27"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="29"/>
-      <c r="B153" s="29"/>
+      <c r="A153" s="27"/>
+      <c r="B153" s="27"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="29"/>
-      <c r="B154" s="29"/>
+      <c r="A154" s="27"/>
+      <c r="B154" s="27"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="29"/>
-      <c r="B155" s="29"/>
+      <c r="A155" s="27"/>
+      <c r="B155" s="27"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="29"/>
-      <c r="B156" s="29"/>
+      <c r="A156" s="27"/>
+      <c r="B156" s="27"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="29"/>
-      <c r="B157" s="29"/>
+      <c r="A157" s="27"/>
+      <c r="B157" s="27"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="29"/>
-      <c r="B158" s="29"/>
+      <c r="A158" s="27"/>
+      <c r="B158" s="27"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="29"/>
-      <c r="B159" s="29"/>
+      <c r="A159" s="27"/>
+      <c r="B159" s="27"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="29"/>
-      <c r="B160" s="29"/>
+      <c r="A160" s="27"/>
+      <c r="B160" s="27"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="29"/>
-      <c r="B161" s="29"/>
+      <c r="A161" s="27"/>
+      <c r="B161" s="27"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="29"/>
-      <c r="B162" s="29"/>
+      <c r="A162" s="27"/>
+      <c r="B162" s="27"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="29"/>
-      <c r="B163" s="29"/>
+      <c r="A163" s="27"/>
+      <c r="B163" s="27"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="29"/>
-      <c r="B164" s="29"/>
+      <c r="A164" s="27"/>
+      <c r="B164" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="145">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A149:B149"/>
     <mergeCell ref="A160:B160"/>
     <mergeCell ref="A161:B161"/>
     <mergeCell ref="A162:B162"/>
@@ -3184,141 +3335,6 @@
     <mergeCell ref="A157:B157"/>
     <mergeCell ref="A158:B158"/>
     <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3348,17 +3364,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
@@ -8881,7 +8897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD668FA6-C86B-4B15-9051-DF984B595504}">
   <dimension ref="A1:I301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -8900,17 +8916,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -11239,17 +11255,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -12902,8 +12918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C04FC45-08E6-489F-B80B-6935CE0BF902}">
   <dimension ref="A1:I300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12921,17 +12937,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -13197,6 +13213,24 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>238</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>595</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>596</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>594</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>597</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -14649,6 +14683,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14675,17 +14710,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
@@ -16526,17 +16561,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -18593,17 +18628,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -20300,20 +20335,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
       <c r="D1" s="17"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="18" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Created MCAD and ECAD Parts
</commit_message>
<xml_diff>
--- a/CougsInSpace-Inventory.xlsx
+++ b/CougsInSpace-Inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\CougsInSpace\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bradley\Documents\CougsInSpace\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63805E8C-90F5-4C7F-8230-21EB7879F443}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E327E13-0788-43D3-A387-E0D1C4988D29}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{42A108CB-A0BE-49ED-8B7A-3FB1AB856735}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="7" xr2:uid="{42A108CB-A0BE-49ED-8B7A-3FB1AB856735}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3504" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3515" uniqueCount="629">
   <si>
     <t>Vendors have been selected by high reputability and lowest price</t>
   </si>
@@ -1901,6 +1901,27 @@
   </si>
   <si>
     <t>399-13212-1-ND</t>
+  </si>
+  <si>
+    <t>30MΩ</t>
+  </si>
+  <si>
+    <t>21-3005</t>
+  </si>
+  <si>
+    <t>CRCW060330M0JPEAHR</t>
+  </si>
+  <si>
+    <t>541-30MAHCT-ND</t>
+  </si>
+  <si>
+    <t>49-0002</t>
+  </si>
+  <si>
+    <t>B3U-1000P</t>
+  </si>
+  <si>
+    <t>SW1020CT-ND</t>
   </si>
 </sst>
 </file>
@@ -1993,7 +2014,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2037,16 +2058,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2058,7 +2080,14 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2440,10 +2469,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="35"/>
       <c r="C1" s="1"/>
       <c r="D1" s="21"/>
       <c r="E1" s="1"/>
@@ -2452,10 +2481,10 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="2"/>
@@ -2465,18 +2494,18 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="7"/>
       <c r="E4" s="7"/>
     </row>
@@ -2584,687 +2613,822 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="32" t="s">
         <v>411</v>
       </c>
-      <c r="B24" s="34"/>
+      <c r="B24" s="32"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="32" t="s">
         <v>412</v>
       </c>
-      <c r="B25" s="34"/>
+      <c r="B25" s="32"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="32" t="s">
         <v>413</v>
       </c>
-      <c r="B26" s="34"/>
+      <c r="B26" s="32"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="32" t="s">
         <v>414</v>
       </c>
-      <c r="B27" s="34"/>
+      <c r="B27" s="32"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="32" t="s">
         <v>415</v>
       </c>
-      <c r="B28" s="34"/>
+      <c r="B28" s="32"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="32" t="s">
         <v>416</v>
       </c>
-      <c r="B29" s="34"/>
+      <c r="B29" s="32"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="32" t="s">
         <v>417</v>
       </c>
-      <c r="B30" s="34"/>
+      <c r="B30" s="32"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="32" t="s">
         <v>418</v>
       </c>
-      <c r="B31" s="34"/>
+      <c r="B31" s="32"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="32" t="s">
         <v>419</v>
       </c>
-      <c r="B32" s="34"/>
+      <c r="B32" s="32"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="32" t="s">
         <v>420</v>
       </c>
-      <c r="B33" s="34"/>
+      <c r="B33" s="32"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="33" t="s">
         <v>516</v>
       </c>
-      <c r="B34" s="35"/>
+      <c r="B34" s="33"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="32" t="s">
         <v>517</v>
       </c>
-      <c r="B35" s="34"/>
+      <c r="B35" s="32"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="32" t="s">
         <v>518</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="32"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="32" t="s">
         <v>519</v>
       </c>
-      <c r="B37" s="34"/>
+      <c r="B37" s="32"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="33" t="s">
         <v>520</v>
       </c>
-      <c r="B38" s="35"/>
+      <c r="B38" s="33"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="33" t="s">
         <v>521</v>
       </c>
-      <c r="B39" s="35"/>
+      <c r="B39" s="33"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="33" t="s">
         <v>514</v>
       </c>
-      <c r="B40" s="35"/>
+      <c r="B40" s="33"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="33" t="s">
         <v>515</v>
       </c>
-      <c r="B41" s="35"/>
+      <c r="B41" s="33"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="33" t="s">
         <v>523</v>
       </c>
-      <c r="B42" s="35"/>
+      <c r="B42" s="33"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="33" t="s">
         <v>527</v>
       </c>
-      <c r="B43" s="35"/>
+      <c r="B43" s="33"/>
     </row>
     <row r="44" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="36" t="s">
+      <c r="A44" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="B44" s="36"/>
+      <c r="B44" s="34"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="34" t="s">
+      <c r="A45" s="32" t="s">
         <v>462</v>
       </c>
-      <c r="B45" s="34"/>
+      <c r="B45" s="32"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="34" t="s">
+      <c r="A46" s="32" t="s">
         <v>463</v>
       </c>
-      <c r="B46" s="34"/>
+      <c r="B46" s="32"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="34" t="s">
+      <c r="A47" s="32" t="s">
         <v>464</v>
       </c>
-      <c r="B47" s="34"/>
+      <c r="B47" s="32"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="34" t="s">
+      <c r="A48" s="32" t="s">
         <v>465</v>
       </c>
-      <c r="B48" s="34"/>
+      <c r="B48" s="32"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="34" t="s">
+      <c r="A49" s="32" t="s">
         <v>466</v>
       </c>
-      <c r="B49" s="34"/>
+      <c r="B49" s="32"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="32" t="s">
         <v>467</v>
       </c>
-      <c r="B50" s="34"/>
+      <c r="B50" s="32"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="34" t="s">
+      <c r="A51" s="32" t="s">
         <v>468</v>
       </c>
-      <c r="B51" s="34"/>
+      <c r="B51" s="32"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="34" t="s">
+      <c r="A52" s="32" t="s">
         <v>469</v>
       </c>
-      <c r="B52" s="34"/>
+      <c r="B52" s="32"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="34" t="s">
+      <c r="A53" s="32" t="s">
         <v>470</v>
       </c>
-      <c r="B53" s="34"/>
+      <c r="B53" s="32"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="34" t="s">
+      <c r="A54" s="32" t="s">
         <v>451</v>
       </c>
-      <c r="B54" s="34"/>
+      <c r="B54" s="32"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="32" t="s">
         <v>452</v>
       </c>
-      <c r="B55" s="34"/>
+      <c r="B55" s="32"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="34" t="s">
+      <c r="A56" s="32" t="s">
         <v>453</v>
       </c>
-      <c r="B56" s="34"/>
+      <c r="B56" s="32"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="33" t="s">
         <v>454</v>
       </c>
-      <c r="B57" s="35"/>
+      <c r="B57" s="33"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="35" t="s">
+      <c r="A58" s="33" t="s">
         <v>455</v>
       </c>
-      <c r="B58" s="35"/>
+      <c r="B58" s="33"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="35" t="s">
+      <c r="A59" s="33" t="s">
         <v>456</v>
       </c>
-      <c r="B59" s="35"/>
+      <c r="B59" s="33"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="35" t="s">
+      <c r="A60" s="33" t="s">
         <v>457</v>
       </c>
-      <c r="B60" s="35"/>
+      <c r="B60" s="33"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="33" t="s">
         <v>458</v>
       </c>
-      <c r="B61" s="35"/>
+      <c r="B61" s="33"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="34" t="s">
+      <c r="A62" s="32" t="s">
         <v>510</v>
       </c>
-      <c r="B62" s="34"/>
+      <c r="B62" s="32"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="34" t="s">
+      <c r="A63" s="32" t="s">
         <v>511</v>
       </c>
-      <c r="B63" s="34"/>
+      <c r="B63" s="32"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="34" t="s">
+      <c r="A64" s="32" t="s">
         <v>488</v>
       </c>
-      <c r="B64" s="34"/>
+      <c r="B64" s="32"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="34" t="s">
+      <c r="A65" s="32" t="s">
         <v>489</v>
       </c>
-      <c r="B65" s="34"/>
+      <c r="B65" s="32"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="34" t="s">
+      <c r="A66" s="32" t="s">
         <v>490</v>
       </c>
-      <c r="B66" s="34"/>
+      <c r="B66" s="32"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="34" t="s">
+      <c r="A67" s="32" t="s">
         <v>491</v>
       </c>
-      <c r="B67" s="34"/>
+      <c r="B67" s="32"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="34" t="s">
+      <c r="A68" s="32" t="s">
         <v>492</v>
       </c>
-      <c r="B68" s="34"/>
+      <c r="B68" s="32"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="34" t="s">
+      <c r="A69" s="32" t="s">
         <v>493</v>
       </c>
-      <c r="B69" s="34"/>
+      <c r="B69" s="32"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="34" t="s">
+      <c r="A70" s="32" t="s">
         <v>494</v>
       </c>
-      <c r="B70" s="34"/>
+      <c r="B70" s="32"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="34" t="s">
+      <c r="A71" s="32" t="s">
         <v>495</v>
       </c>
-      <c r="B71" s="34"/>
+      <c r="B71" s="32"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="34" t="s">
+      <c r="A72" s="32" t="s">
         <v>496</v>
       </c>
-      <c r="B72" s="34"/>
+      <c r="B72" s="32"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="34" t="s">
+      <c r="A73" s="32" t="s">
         <v>497</v>
       </c>
-      <c r="B73" s="34"/>
+      <c r="B73" s="32"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="35" t="s">
+      <c r="A74" s="33" t="s">
         <v>529</v>
       </c>
-      <c r="B74" s="35"/>
+      <c r="B74" s="33"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="35" t="s">
+      <c r="A75" s="33" t="s">
         <v>530</v>
       </c>
-      <c r="B75" s="35"/>
+      <c r="B75" s="33"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="35" t="s">
+      <c r="A76" s="33" t="s">
         <v>552</v>
       </c>
-      <c r="B76" s="35"/>
+      <c r="B76" s="33"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="35" t="s">
+      <c r="A77" s="33" t="s">
         <v>531</v>
       </c>
-      <c r="B77" s="35"/>
+      <c r="B77" s="33"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="35" t="s">
+      <c r="A78" s="33" t="s">
         <v>532</v>
       </c>
-      <c r="B78" s="35"/>
+      <c r="B78" s="33"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="35" t="s">
+      <c r="A79" s="33" t="s">
         <v>533</v>
       </c>
-      <c r="B79" s="35"/>
+      <c r="B79" s="33"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="35" t="s">
+      <c r="A80" s="33" t="s">
         <v>534</v>
       </c>
-      <c r="B80" s="35"/>
+      <c r="B80" s="33"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="35" t="s">
+      <c r="A81" s="33" t="s">
         <v>535</v>
       </c>
-      <c r="B81" s="35"/>
+      <c r="B81" s="33"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="34"/>
-      <c r="B82" s="34"/>
+      <c r="A82" s="32"/>
+      <c r="B82" s="32"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="34"/>
-      <c r="B83" s="34"/>
+      <c r="A83" s="32"/>
+      <c r="B83" s="32"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="34"/>
-      <c r="B84" s="34"/>
+      <c r="A84" s="32"/>
+      <c r="B84" s="32"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="34"/>
-      <c r="B85" s="34"/>
+      <c r="A85" s="32"/>
+      <c r="B85" s="32"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="34"/>
-      <c r="B86" s="34"/>
+      <c r="A86" s="32"/>
+      <c r="B86" s="32"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="34"/>
-      <c r="B87" s="34"/>
+      <c r="A87" s="32"/>
+      <c r="B87" s="32"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="34"/>
-      <c r="B88" s="34"/>
+      <c r="A88" s="32"/>
+      <c r="B88" s="32"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="34"/>
-      <c r="B89" s="34"/>
+      <c r="A89" s="32"/>
+      <c r="B89" s="32"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="34"/>
-      <c r="B90" s="34"/>
+      <c r="A90" s="32"/>
+      <c r="B90" s="32"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="34"/>
-      <c r="B91" s="34"/>
+      <c r="A91" s="32"/>
+      <c r="B91" s="32"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="34"/>
-      <c r="B92" s="34"/>
+      <c r="A92" s="32"/>
+      <c r="B92" s="32"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="34"/>
-      <c r="B93" s="34"/>
+      <c r="A93" s="32"/>
+      <c r="B93" s="32"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="34"/>
-      <c r="B94" s="34"/>
+      <c r="A94" s="32"/>
+      <c r="B94" s="32"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="34"/>
-      <c r="B95" s="34"/>
+      <c r="A95" s="32"/>
+      <c r="B95" s="32"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="34"/>
-      <c r="B96" s="34"/>
+      <c r="A96" s="32"/>
+      <c r="B96" s="32"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="34"/>
-      <c r="B97" s="34"/>
+      <c r="A97" s="32"/>
+      <c r="B97" s="32"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="34"/>
-      <c r="B98" s="34"/>
+      <c r="A98" s="32"/>
+      <c r="B98" s="32"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="34"/>
-      <c r="B99" s="34"/>
+      <c r="A99" s="32"/>
+      <c r="B99" s="32"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="34"/>
-      <c r="B100" s="34"/>
+      <c r="A100" s="32"/>
+      <c r="B100" s="32"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="34"/>
-      <c r="B101" s="34"/>
+      <c r="A101" s="32"/>
+      <c r="B101" s="32"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="34"/>
-      <c r="B102" s="34"/>
+      <c r="A102" s="32"/>
+      <c r="B102" s="32"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="34"/>
-      <c r="B103" s="34"/>
+      <c r="A103" s="32"/>
+      <c r="B103" s="32"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="34"/>
-      <c r="B104" s="34"/>
+      <c r="A104" s="32"/>
+      <c r="B104" s="32"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="34"/>
-      <c r="B105" s="34"/>
+      <c r="A105" s="32"/>
+      <c r="B105" s="32"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="34"/>
-      <c r="B106" s="34"/>
+      <c r="A106" s="32"/>
+      <c r="B106" s="32"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="34"/>
-      <c r="B107" s="34"/>
+      <c r="A107" s="32"/>
+      <c r="B107" s="32"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="34"/>
-      <c r="B108" s="34"/>
+      <c r="A108" s="32"/>
+      <c r="B108" s="32"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="34"/>
-      <c r="B109" s="34"/>
+      <c r="A109" s="32"/>
+      <c r="B109" s="32"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="34"/>
-      <c r="B110" s="34"/>
+      <c r="A110" s="32"/>
+      <c r="B110" s="32"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="34"/>
-      <c r="B111" s="34"/>
+      <c r="A111" s="32"/>
+      <c r="B111" s="32"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="34"/>
-      <c r="B112" s="34"/>
+      <c r="A112" s="32"/>
+      <c r="B112" s="32"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="34"/>
-      <c r="B113" s="34"/>
+      <c r="A113" s="32"/>
+      <c r="B113" s="32"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="34"/>
-      <c r="B114" s="34"/>
+      <c r="A114" s="32"/>
+      <c r="B114" s="32"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="34"/>
-      <c r="B115" s="34"/>
+      <c r="A115" s="32"/>
+      <c r="B115" s="32"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="34"/>
-      <c r="B116" s="34"/>
+      <c r="A116" s="32"/>
+      <c r="B116" s="32"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="34"/>
-      <c r="B117" s="34"/>
+      <c r="A117" s="32"/>
+      <c r="B117" s="32"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="34"/>
-      <c r="B118" s="34"/>
+      <c r="A118" s="32"/>
+      <c r="B118" s="32"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="34"/>
-      <c r="B119" s="34"/>
+      <c r="A119" s="32"/>
+      <c r="B119" s="32"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="34"/>
-      <c r="B120" s="34"/>
+      <c r="A120" s="32"/>
+      <c r="B120" s="32"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="34"/>
-      <c r="B121" s="34"/>
+      <c r="A121" s="32"/>
+      <c r="B121" s="32"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="34"/>
-      <c r="B122" s="34"/>
+      <c r="A122" s="32"/>
+      <c r="B122" s="32"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="34"/>
-      <c r="B123" s="34"/>
+      <c r="A123" s="32"/>
+      <c r="B123" s="32"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="34"/>
-      <c r="B124" s="34"/>
+      <c r="A124" s="32"/>
+      <c r="B124" s="32"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="34"/>
-      <c r="B125" s="34"/>
+      <c r="A125" s="32"/>
+      <c r="B125" s="32"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="34"/>
-      <c r="B126" s="34"/>
+      <c r="A126" s="32"/>
+      <c r="B126" s="32"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="34"/>
-      <c r="B127" s="34"/>
+      <c r="A127" s="32"/>
+      <c r="B127" s="32"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="34"/>
-      <c r="B128" s="34"/>
+      <c r="A128" s="32"/>
+      <c r="B128" s="32"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="34"/>
-      <c r="B129" s="34"/>
+      <c r="A129" s="32"/>
+      <c r="B129" s="32"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="34"/>
-      <c r="B130" s="34"/>
+      <c r="A130" s="32"/>
+      <c r="B130" s="32"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="34"/>
-      <c r="B131" s="34"/>
+      <c r="A131" s="32"/>
+      <c r="B131" s="32"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="34"/>
-      <c r="B132" s="34"/>
+      <c r="A132" s="32"/>
+      <c r="B132" s="32"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="34"/>
-      <c r="B133" s="34"/>
+      <c r="A133" s="32"/>
+      <c r="B133" s="32"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="34"/>
-      <c r="B134" s="34"/>
+      <c r="A134" s="32"/>
+      <c r="B134" s="32"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="34"/>
-      <c r="B135" s="34"/>
+      <c r="A135" s="32"/>
+      <c r="B135" s="32"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="34"/>
-      <c r="B136" s="34"/>
+      <c r="A136" s="32"/>
+      <c r="B136" s="32"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="34"/>
-      <c r="B137" s="34"/>
+      <c r="A137" s="32"/>
+      <c r="B137" s="32"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="34"/>
-      <c r="B138" s="34"/>
+      <c r="A138" s="32"/>
+      <c r="B138" s="32"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="34"/>
-      <c r="B139" s="34"/>
+      <c r="A139" s="32"/>
+      <c r="B139" s="32"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="34"/>
-      <c r="B140" s="34"/>
+      <c r="A140" s="32"/>
+      <c r="B140" s="32"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="34"/>
-      <c r="B141" s="34"/>
+      <c r="A141" s="32"/>
+      <c r="B141" s="32"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="34"/>
-      <c r="B142" s="34"/>
+      <c r="A142" s="32"/>
+      <c r="B142" s="32"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="34"/>
-      <c r="B143" s="34"/>
+      <c r="A143" s="32"/>
+      <c r="B143" s="32"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="34"/>
-      <c r="B144" s="34"/>
+      <c r="A144" s="32"/>
+      <c r="B144" s="32"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="34"/>
-      <c r="B145" s="34"/>
+      <c r="A145" s="32"/>
+      <c r="B145" s="32"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="34"/>
-      <c r="B146" s="34"/>
+      <c r="A146" s="32"/>
+      <c r="B146" s="32"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="34"/>
-      <c r="B147" s="34"/>
+      <c r="A147" s="32"/>
+      <c r="B147" s="32"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="34"/>
-      <c r="B148" s="34"/>
+      <c r="A148" s="32"/>
+      <c r="B148" s="32"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="34"/>
-      <c r="B149" s="34"/>
+      <c r="A149" s="32"/>
+      <c r="B149" s="32"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="34"/>
-      <c r="B150" s="34"/>
+      <c r="A150" s="32"/>
+      <c r="B150" s="32"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="34"/>
-      <c r="B151" s="34"/>
+      <c r="A151" s="32"/>
+      <c r="B151" s="32"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="34"/>
-      <c r="B152" s="34"/>
+      <c r="A152" s="32"/>
+      <c r="B152" s="32"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="34"/>
-      <c r="B153" s="34"/>
+      <c r="A153" s="32"/>
+      <c r="B153" s="32"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="34"/>
-      <c r="B154" s="34"/>
+      <c r="A154" s="32"/>
+      <c r="B154" s="32"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="34"/>
-      <c r="B155" s="34"/>
+      <c r="A155" s="32"/>
+      <c r="B155" s="32"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="34"/>
-      <c r="B156" s="34"/>
+      <c r="A156" s="32"/>
+      <c r="B156" s="32"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="34"/>
-      <c r="B157" s="34"/>
+      <c r="A157" s="32"/>
+      <c r="B157" s="32"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="34"/>
-      <c r="B158" s="34"/>
+      <c r="A158" s="32"/>
+      <c r="B158" s="32"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="34"/>
-      <c r="B159" s="34"/>
+      <c r="A159" s="32"/>
+      <c r="B159" s="32"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="34"/>
-      <c r="B160" s="34"/>
+      <c r="A160" s="32"/>
+      <c r="B160" s="32"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="34"/>
-      <c r="B161" s="34"/>
+      <c r="A161" s="32"/>
+      <c r="B161" s="32"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="34"/>
-      <c r="B162" s="34"/>
+      <c r="A162" s="32"/>
+      <c r="B162" s="32"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="34"/>
-      <c r="B163" s="34"/>
+      <c r="A163" s="32"/>
+      <c r="B163" s="32"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="34"/>
-      <c r="B164" s="34"/>
+      <c r="A164" s="32"/>
+      <c r="B164" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="145">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A149:B149"/>
     <mergeCell ref="A160:B160"/>
     <mergeCell ref="A161:B161"/>
     <mergeCell ref="A162:B162"/>
@@ -3275,141 +3439,6 @@
     <mergeCell ref="A157:B157"/>
     <mergeCell ref="A158:B158"/>
     <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3439,17 +3468,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
@@ -8981,7 +9010,7 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C1001">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8992,10 +9021,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD668FA6-C86B-4B15-9051-DF984B595504}">
-  <dimension ref="A1:I302"/>
+  <dimension ref="A1:I303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9013,17 +9042,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -9057,7 +9086,7 @@
     <row r="4" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30"/>
       <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="28" t="s">
         <v>615</v>
       </c>
@@ -9570,91 +9599,83 @@
         <v>361</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
-        <v>4</v>
-      </c>
-      <c r="B22" s="10">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2">
-        <v>4</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>374</v>
+    <row r="22" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="2"/>
+      <c r="D22" s="31" t="s">
+        <v>622</v>
       </c>
       <c r="E22" s="5">
         <v>1608</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>578</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H22" s="10" t="s">
+        <v>623</v>
+      </c>
+      <c r="G22" s="31" t="s">
+        <v>624</v>
+      </c>
+      <c r="H22" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="I22" s="10" t="s">
-        <v>125</v>
+      <c r="I22" s="31" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" s="10">
         <v>0</v>
       </c>
       <c r="C23" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E23" s="5">
         <v>1608</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>570</v>
+        <v>578</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B24" s="10">
         <v>0</v>
       </c>
       <c r="C24" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>297</v>
+        <v>375</v>
       </c>
       <c r="E24" s="5">
         <v>1608</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>298</v>
+        <v>116</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>146</v>
+        <v>6</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>299</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -9668,346 +9689,370 @@
         <v>8</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="E25" s="5">
         <v>1608</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="H25" s="10" t="s">
         <v>146</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" s="10">
         <v>0</v>
       </c>
       <c r="C26" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>342</v>
+        <v>288</v>
       </c>
       <c r="E26" s="5">
         <v>1608</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>343</v>
+        <v>289</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>344</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B27" s="10">
         <v>0</v>
       </c>
       <c r="C27" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>279</v>
+        <v>342</v>
       </c>
       <c r="E27" s="5">
         <v>1608</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>572</v>
+        <v>580</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>280</v>
+        <v>343</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>281</v>
+        <v>344</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B28" s="10">
         <v>0</v>
       </c>
       <c r="C28" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>376</v>
+        <v>279</v>
       </c>
       <c r="E28" s="5">
         <v>1608</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>581</v>
+        <v>572</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>126</v>
+        <v>280</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>127</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B29" s="10">
         <v>0</v>
       </c>
       <c r="C29" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E29" s="5">
         <v>1608</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="H29" s="10" t="s">
         <v>101</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B30" s="10">
         <v>0</v>
       </c>
       <c r="C30" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E30" s="5">
         <v>1608</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B31" s="10">
         <v>0</v>
       </c>
       <c r="C31" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E31" s="5">
         <v>1608</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B32" s="10">
         <v>0</v>
       </c>
       <c r="C32" s="2">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>237</v>
+        <v>379</v>
       </c>
       <c r="E32" s="5">
         <v>1608</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>235</v>
+        <v>132</v>
       </c>
       <c r="H32" s="10" t="s">
         <v>101</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>236</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B33" s="10">
         <v>0</v>
       </c>
       <c r="C33" s="2">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>300</v>
+        <v>237</v>
       </c>
       <c r="E33" s="5">
         <v>1608</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>577</v>
+        <v>585</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>301</v>
+        <v>235</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="I33" s="10" t="s">
-        <v>302</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B34" s="10">
         <v>0</v>
       </c>
       <c r="C34" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>380</v>
+        <v>300</v>
       </c>
       <c r="E34" s="5">
         <v>1608</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>120</v>
+        <v>301</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>121</v>
+        <v>302</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B35" s="10">
         <v>0</v>
       </c>
       <c r="C35" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>111</v>
+        <v>380</v>
+      </c>
+      <c r="E35" s="5">
+        <v>1608</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B36" s="10">
         <v>0</v>
       </c>
       <c r="C36" s="2">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>303</v>
-      </c>
-      <c r="E36" s="5">
-        <v>1608</v>
+        <v>109</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>592</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>303</v>
+        <v>593</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>146</v>
       </c>
       <c r="I36" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>21</v>
+      </c>
+      <c r="B37" s="10">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>13</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="E37" s="5">
+        <v>1608</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="I37" s="10" t="s">
         <v>304</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C37" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -11335,20 +11380,31 @@
         <v>238</v>
       </c>
     </row>
+    <row r="303" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C303" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A5:I46">
-    <sortCondition ref="D5:D46"/>
-    <sortCondition ref="E5:E46"/>
+  <sortState ref="A5:I47">
+    <sortCondition ref="D5:D47"/>
+    <sortCondition ref="E5:E47"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:C302">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+  <conditionalFormatting sqref="C5:C303">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11375,17 +11431,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -13026,7 +13082,7 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C300">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13057,17 +13113,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -14834,7 +14890,7 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C300">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14866,17 +14922,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
@@ -16721,7 +16777,7 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C299">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16753,17 +16809,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -18788,7 +18844,7 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C300">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18801,8 +18857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B93B4E-C631-4E38-89FB-3745EC8A8869}">
   <dimension ref="A1:I300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18820,17 +18876,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -19047,6 +19103,24 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>238</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>627</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>627</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>626</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>627</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -20499,7 +20573,7 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C300">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20527,20 +20601,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="17"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
       <c r="D2" s="18" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Added Bussed Resistor Network
</commit_message>
<xml_diff>
--- a/CougsInSpace-Inventory.xlsx
+++ b/CougsInSpace-Inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bradley\Documents\CougsInSpace\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\GitHub\CougsInSpace\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441DB62C-7A13-4F7C-B0E2-4AFCD725F274}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994EDCA0-46A2-4A35-87AD-867558C2E722}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3" xr2:uid="{42A108CB-A0BE-49ED-8B7A-3FB1AB856735}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{42A108CB-A0BE-49ED-8B7A-3FB1AB856735}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Other" sheetId="14" r:id="rId8"/>
     <sheet name="Equipment" sheetId="5" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3542" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3548" uniqueCount="652">
   <si>
     <t>Vendors have been selected by high reputability and lowest price</t>
   </si>
@@ -1807,18 +1807,6 @@
     <t>25-10.0</t>
   </si>
   <si>
-    <t>26-1002</t>
-  </si>
-  <si>
-    <t>26-2203</t>
-  </si>
-  <si>
-    <t>26-6802</t>
-  </si>
-  <si>
-    <t>26-3001</t>
-  </si>
-  <si>
     <t>04-0006</t>
   </si>
   <si>
@@ -1979,6 +1967,30 @@
   </si>
   <si>
     <t>81-LQM18PN4R7MFRL</t>
+  </si>
+  <si>
+    <t>3264</t>
+  </si>
+  <si>
+    <t>26-0000</t>
+  </si>
+  <si>
+    <t>26-0001</t>
+  </si>
+  <si>
+    <t>26-0002</t>
+  </si>
+  <si>
+    <t>26-0003</t>
+  </si>
+  <si>
+    <t>26-0004</t>
+  </si>
+  <si>
+    <t>YC358TJK-0710KL</t>
+  </si>
+  <si>
+    <t>YC358T-10KCT-ND</t>
   </si>
 </sst>
 </file>
@@ -2071,7 +2083,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2119,15 +2131,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2516,7 +2529,7 @@
   <dimension ref="A1:J164"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="10" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="bottomLeft" activeCell="A70" sqref="A70:B70"/>
     </sheetView>
@@ -2528,10 +2541,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="35"/>
       <c r="C1" s="1"/>
       <c r="D1" s="21"/>
       <c r="E1" s="1"/>
@@ -2540,10 +2553,10 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="2"/>
@@ -2553,18 +2566,18 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="39"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="39"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="7"/>
       <c r="E4" s="7"/>
     </row>
@@ -2672,732 +2685,777 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="38" t="s">
         <v>411</v>
       </c>
-      <c r="B24" s="34"/>
+      <c r="B24" s="38"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="38" t="s">
         <v>412</v>
       </c>
-      <c r="B25" s="34"/>
+      <c r="B25" s="38"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="38" t="s">
         <v>413</v>
       </c>
-      <c r="B26" s="34"/>
+      <c r="B26" s="38"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="38" t="s">
         <v>414</v>
       </c>
-      <c r="B27" s="34"/>
+      <c r="B27" s="38"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="38" t="s">
         <v>415</v>
       </c>
-      <c r="B28" s="34"/>
+      <c r="B28" s="38"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="38" t="s">
         <v>416</v>
       </c>
-      <c r="B29" s="34"/>
+      <c r="B29" s="38"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="38" t="s">
         <v>417</v>
       </c>
-      <c r="B30" s="34"/>
+      <c r="B30" s="38"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="38" t="s">
         <v>418</v>
       </c>
-      <c r="B31" s="34"/>
+      <c r="B31" s="38"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="38" t="s">
         <v>419</v>
       </c>
-      <c r="B32" s="34"/>
+      <c r="B32" s="38"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="38" t="s">
         <v>420</v>
       </c>
-      <c r="B33" s="34"/>
+      <c r="B33" s="38"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="39" t="s">
         <v>516</v>
       </c>
-      <c r="B34" s="35"/>
+      <c r="B34" s="39"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="38" t="s">
         <v>517</v>
       </c>
-      <c r="B35" s="34"/>
+      <c r="B35" s="38"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="38" t="s">
         <v>518</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="38"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="38" t="s">
         <v>519</v>
       </c>
-      <c r="B37" s="34"/>
+      <c r="B37" s="38"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="39" t="s">
         <v>520</v>
       </c>
-      <c r="B38" s="35"/>
+      <c r="B38" s="39"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="39" t="s">
         <v>521</v>
       </c>
-      <c r="B39" s="35"/>
+      <c r="B39" s="39"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="39" t="s">
         <v>514</v>
       </c>
-      <c r="B40" s="35"/>
+      <c r="B40" s="39"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="39" t="s">
         <v>515</v>
       </c>
-      <c r="B41" s="35"/>
+      <c r="B41" s="39"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="39" t="s">
         <v>523</v>
       </c>
-      <c r="B42" s="35"/>
+      <c r="B42" s="39"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="39" t="s">
         <v>527</v>
       </c>
-      <c r="B43" s="35"/>
+      <c r="B43" s="39"/>
     </row>
     <row r="44" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="36" t="s">
+      <c r="A44" s="40" t="s">
         <v>471</v>
       </c>
-      <c r="B44" s="36"/>
+      <c r="B44" s="40"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="34" t="s">
+      <c r="A45" s="38" t="s">
         <v>462</v>
       </c>
-      <c r="B45" s="34"/>
+      <c r="B45" s="38"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="34" t="s">
+      <c r="A46" s="38" t="s">
         <v>463</v>
       </c>
-      <c r="B46" s="34"/>
+      <c r="B46" s="38"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="34" t="s">
+      <c r="A47" s="38" t="s">
         <v>464</v>
       </c>
-      <c r="B47" s="34"/>
+      <c r="B47" s="38"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="34" t="s">
+      <c r="A48" s="38" t="s">
         <v>465</v>
       </c>
-      <c r="B48" s="34"/>
+      <c r="B48" s="38"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="34" t="s">
+      <c r="A49" s="38" t="s">
         <v>466</v>
       </c>
-      <c r="B49" s="34"/>
+      <c r="B49" s="38"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="38" t="s">
         <v>467</v>
       </c>
-      <c r="B50" s="34"/>
+      <c r="B50" s="38"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="34" t="s">
+      <c r="A51" s="38" t="s">
         <v>468</v>
       </c>
-      <c r="B51" s="34"/>
+      <c r="B51" s="38"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="34" t="s">
+      <c r="A52" s="38" t="s">
         <v>469</v>
       </c>
-      <c r="B52" s="34"/>
+      <c r="B52" s="38"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="34" t="s">
+      <c r="A53" s="38" t="s">
         <v>470</v>
       </c>
-      <c r="B53" s="34"/>
+      <c r="B53" s="38"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="34" t="s">
+      <c r="A54" s="38" t="s">
         <v>451</v>
       </c>
-      <c r="B54" s="34"/>
+      <c r="B54" s="38"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="38" t="s">
         <v>452</v>
       </c>
-      <c r="B55" s="34"/>
+      <c r="B55" s="38"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="34" t="s">
+      <c r="A56" s="38" t="s">
         <v>453</v>
       </c>
-      <c r="B56" s="34"/>
+      <c r="B56" s="38"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="39" t="s">
         <v>454</v>
       </c>
-      <c r="B57" s="35"/>
+      <c r="B57" s="39"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="35" t="s">
+      <c r="A58" s="39" t="s">
         <v>455</v>
       </c>
-      <c r="B58" s="35"/>
+      <c r="B58" s="39"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="35" t="s">
+      <c r="A59" s="39" t="s">
         <v>456</v>
       </c>
-      <c r="B59" s="35"/>
+      <c r="B59" s="39"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="35" t="s">
+      <c r="A60" s="39" t="s">
         <v>457</v>
       </c>
-      <c r="B60" s="35"/>
+      <c r="B60" s="39"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="39" t="s">
         <v>458</v>
       </c>
-      <c r="B61" s="35"/>
+      <c r="B61" s="39"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="34" t="s">
+      <c r="A62" s="38" t="s">
         <v>510</v>
       </c>
-      <c r="B62" s="34"/>
+      <c r="B62" s="38"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="34" t="s">
+      <c r="A63" s="38" t="s">
         <v>511</v>
       </c>
-      <c r="B63" s="34"/>
+      <c r="B63" s="38"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="34" t="s">
+      <c r="A64" s="38" t="s">
         <v>488</v>
       </c>
-      <c r="B64" s="34"/>
+      <c r="B64" s="38"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="34" t="s">
+      <c r="A65" s="38" t="s">
         <v>489</v>
       </c>
-      <c r="B65" s="34"/>
+      <c r="B65" s="38"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="34" t="s">
+      <c r="A66" s="38" t="s">
         <v>490</v>
       </c>
-      <c r="B66" s="34"/>
+      <c r="B66" s="38"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="34" t="s">
+      <c r="A67" s="38" t="s">
         <v>491</v>
       </c>
-      <c r="B67" s="34"/>
+      <c r="B67" s="38"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="34" t="s">
+      <c r="A68" s="38" t="s">
         <v>492</v>
       </c>
-      <c r="B68" s="34"/>
+      <c r="B68" s="38"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="34" t="s">
+      <c r="A69" s="38" t="s">
         <v>493</v>
       </c>
-      <c r="B69" s="34"/>
+      <c r="B69" s="38"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="34" t="s">
+      <c r="A70" s="38" t="s">
         <v>494</v>
       </c>
-      <c r="B70" s="34"/>
+      <c r="B70" s="38"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="34" t="s">
+      <c r="A71" s="38" t="s">
         <v>495</v>
       </c>
-      <c r="B71" s="34"/>
+      <c r="B71" s="38"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="34" t="s">
+      <c r="A72" s="38" t="s">
         <v>496</v>
       </c>
-      <c r="B72" s="34"/>
+      <c r="B72" s="38"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="34" t="s">
+      <c r="A73" s="38" t="s">
         <v>497</v>
       </c>
-      <c r="B73" s="34"/>
+      <c r="B73" s="38"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="35" t="s">
+      <c r="A74" s="39" t="s">
         <v>529</v>
       </c>
-      <c r="B74" s="35"/>
+      <c r="B74" s="39"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="35" t="s">
+      <c r="A75" s="39" t="s">
         <v>530</v>
       </c>
-      <c r="B75" s="35"/>
+      <c r="B75" s="39"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="35" t="s">
+      <c r="A76" s="39" t="s">
         <v>552</v>
       </c>
-      <c r="B76" s="35"/>
+      <c r="B76" s="39"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="35" t="s">
+      <c r="A77" s="39" t="s">
         <v>531</v>
       </c>
-      <c r="B77" s="35"/>
+      <c r="B77" s="39"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="35" t="s">
+      <c r="A78" s="39" t="s">
         <v>532</v>
       </c>
-      <c r="B78" s="35"/>
+      <c r="B78" s="39"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="35" t="s">
+      <c r="A79" s="39" t="s">
         <v>533</v>
       </c>
-      <c r="B79" s="35"/>
+      <c r="B79" s="39"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="35" t="s">
+      <c r="A80" s="39" t="s">
         <v>534</v>
       </c>
-      <c r="B80" s="35"/>
+      <c r="B80" s="39"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="35" t="s">
+      <c r="A81" s="39" t="s">
         <v>535</v>
       </c>
-      <c r="B81" s="35"/>
+      <c r="B81" s="39"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="34"/>
-      <c r="B82" s="34"/>
+      <c r="A82" s="38"/>
+      <c r="B82" s="38"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="34"/>
-      <c r="B83" s="34"/>
+      <c r="A83" s="38"/>
+      <c r="B83" s="38"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="34"/>
-      <c r="B84" s="34"/>
+      <c r="A84" s="38"/>
+      <c r="B84" s="38"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="34"/>
-      <c r="B85" s="34"/>
+      <c r="A85" s="38"/>
+      <c r="B85" s="38"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="34"/>
-      <c r="B86" s="34"/>
+      <c r="A86" s="38"/>
+      <c r="B86" s="38"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="34"/>
-      <c r="B87" s="34"/>
+      <c r="A87" s="38"/>
+      <c r="B87" s="38"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="34"/>
-      <c r="B88" s="34"/>
+      <c r="A88" s="38"/>
+      <c r="B88" s="38"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="34"/>
-      <c r="B89" s="34"/>
+      <c r="A89" s="38"/>
+      <c r="B89" s="38"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="34"/>
-      <c r="B90" s="34"/>
+      <c r="A90" s="38"/>
+      <c r="B90" s="38"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="34"/>
-      <c r="B91" s="34"/>
+      <c r="A91" s="38"/>
+      <c r="B91" s="38"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="34"/>
-      <c r="B92" s="34"/>
+      <c r="A92" s="38"/>
+      <c r="B92" s="38"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="34"/>
-      <c r="B93" s="34"/>
+      <c r="A93" s="38"/>
+      <c r="B93" s="38"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="34"/>
-      <c r="B94" s="34"/>
+      <c r="A94" s="38"/>
+      <c r="B94" s="38"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="34"/>
-      <c r="B95" s="34"/>
+      <c r="A95" s="38"/>
+      <c r="B95" s="38"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="34"/>
-      <c r="B96" s="34"/>
+      <c r="A96" s="38"/>
+      <c r="B96" s="38"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="34"/>
-      <c r="B97" s="34"/>
+      <c r="A97" s="38"/>
+      <c r="B97" s="38"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="34"/>
-      <c r="B98" s="34"/>
+      <c r="A98" s="38"/>
+      <c r="B98" s="38"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="34"/>
-      <c r="B99" s="34"/>
+      <c r="A99" s="38"/>
+      <c r="B99" s="38"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="34"/>
-      <c r="B100" s="34"/>
+      <c r="A100" s="38"/>
+      <c r="B100" s="38"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="34"/>
-      <c r="B101" s="34"/>
+      <c r="A101" s="38"/>
+      <c r="B101" s="38"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="34"/>
-      <c r="B102" s="34"/>
+      <c r="A102" s="38"/>
+      <c r="B102" s="38"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="34"/>
-      <c r="B103" s="34"/>
+      <c r="A103" s="38"/>
+      <c r="B103" s="38"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="34"/>
-      <c r="B104" s="34"/>
+      <c r="A104" s="38"/>
+      <c r="B104" s="38"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="34"/>
-      <c r="B105" s="34"/>
+      <c r="A105" s="38"/>
+      <c r="B105" s="38"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="34"/>
-      <c r="B106" s="34"/>
+      <c r="A106" s="38"/>
+      <c r="B106" s="38"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="34"/>
-      <c r="B107" s="34"/>
+      <c r="A107" s="38"/>
+      <c r="B107" s="38"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="34"/>
-      <c r="B108" s="34"/>
+      <c r="A108" s="38"/>
+      <c r="B108" s="38"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="34"/>
-      <c r="B109" s="34"/>
+      <c r="A109" s="38"/>
+      <c r="B109" s="38"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="34"/>
-      <c r="B110" s="34"/>
+      <c r="A110" s="38"/>
+      <c r="B110" s="38"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="34"/>
-      <c r="B111" s="34"/>
+      <c r="A111" s="38"/>
+      <c r="B111" s="38"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="34"/>
-      <c r="B112" s="34"/>
+      <c r="A112" s="38"/>
+      <c r="B112" s="38"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="34"/>
-      <c r="B113" s="34"/>
+      <c r="A113" s="38"/>
+      <c r="B113" s="38"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="34"/>
-      <c r="B114" s="34"/>
+      <c r="A114" s="38"/>
+      <c r="B114" s="38"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="34"/>
-      <c r="B115" s="34"/>
+      <c r="A115" s="38"/>
+      <c r="B115" s="38"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="34"/>
-      <c r="B116" s="34"/>
+      <c r="A116" s="38"/>
+      <c r="B116" s="38"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="34"/>
-      <c r="B117" s="34"/>
+      <c r="A117" s="38"/>
+      <c r="B117" s="38"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="34"/>
-      <c r="B118" s="34"/>
+      <c r="A118" s="38"/>
+      <c r="B118" s="38"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="34"/>
-      <c r="B119" s="34"/>
+      <c r="A119" s="38"/>
+      <c r="B119" s="38"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="34"/>
-      <c r="B120" s="34"/>
+      <c r="A120" s="38"/>
+      <c r="B120" s="38"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="34"/>
-      <c r="B121" s="34"/>
+      <c r="A121" s="38"/>
+      <c r="B121" s="38"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="34"/>
-      <c r="B122" s="34"/>
+      <c r="A122" s="38"/>
+      <c r="B122" s="38"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="34"/>
-      <c r="B123" s="34"/>
+      <c r="A123" s="38"/>
+      <c r="B123" s="38"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="34"/>
-      <c r="B124" s="34"/>
+      <c r="A124" s="38"/>
+      <c r="B124" s="38"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="34"/>
-      <c r="B125" s="34"/>
+      <c r="A125" s="38"/>
+      <c r="B125" s="38"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="34"/>
-      <c r="B126" s="34"/>
+      <c r="A126" s="38"/>
+      <c r="B126" s="38"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="34"/>
-      <c r="B127" s="34"/>
+      <c r="A127" s="38"/>
+      <c r="B127" s="38"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="34"/>
-      <c r="B128" s="34"/>
+      <c r="A128" s="38"/>
+      <c r="B128" s="38"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="34"/>
-      <c r="B129" s="34"/>
+      <c r="A129" s="38"/>
+      <c r="B129" s="38"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="34"/>
-      <c r="B130" s="34"/>
+      <c r="A130" s="38"/>
+      <c r="B130" s="38"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="34"/>
-      <c r="B131" s="34"/>
+      <c r="A131" s="38"/>
+      <c r="B131" s="38"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="34"/>
-      <c r="B132" s="34"/>
+      <c r="A132" s="38"/>
+      <c r="B132" s="38"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="34"/>
-      <c r="B133" s="34"/>
+      <c r="A133" s="38"/>
+      <c r="B133" s="38"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="34"/>
-      <c r="B134" s="34"/>
+      <c r="A134" s="38"/>
+      <c r="B134" s="38"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="34"/>
-      <c r="B135" s="34"/>
+      <c r="A135" s="38"/>
+      <c r="B135" s="38"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="34"/>
-      <c r="B136" s="34"/>
+      <c r="A136" s="38"/>
+      <c r="B136" s="38"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="34"/>
-      <c r="B137" s="34"/>
+      <c r="A137" s="38"/>
+      <c r="B137" s="38"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="34"/>
-      <c r="B138" s="34"/>
+      <c r="A138" s="38"/>
+      <c r="B138" s="38"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="34"/>
-      <c r="B139" s="34"/>
+      <c r="A139" s="38"/>
+      <c r="B139" s="38"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="34"/>
-      <c r="B140" s="34"/>
+      <c r="A140" s="38"/>
+      <c r="B140" s="38"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="34"/>
-      <c r="B141" s="34"/>
+      <c r="A141" s="38"/>
+      <c r="B141" s="38"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="34"/>
-      <c r="B142" s="34"/>
+      <c r="A142" s="38"/>
+      <c r="B142" s="38"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="34"/>
-      <c r="B143" s="34"/>
+      <c r="A143" s="38"/>
+      <c r="B143" s="38"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="34"/>
-      <c r="B144" s="34"/>
+      <c r="A144" s="38"/>
+      <c r="B144" s="38"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="34"/>
-      <c r="B145" s="34"/>
+      <c r="A145" s="38"/>
+      <c r="B145" s="38"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="34"/>
-      <c r="B146" s="34"/>
+      <c r="A146" s="38"/>
+      <c r="B146" s="38"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="34"/>
-      <c r="B147" s="34"/>
+      <c r="A147" s="38"/>
+      <c r="B147" s="38"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="34"/>
-      <c r="B148" s="34"/>
+      <c r="A148" s="38"/>
+      <c r="B148" s="38"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="34"/>
-      <c r="B149" s="34"/>
+      <c r="A149" s="38"/>
+      <c r="B149" s="38"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="34"/>
-      <c r="B150" s="34"/>
+      <c r="A150" s="38"/>
+      <c r="B150" s="38"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="34"/>
-      <c r="B151" s="34"/>
+      <c r="A151" s="38"/>
+      <c r="B151" s="38"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="34"/>
-      <c r="B152" s="34"/>
+      <c r="A152" s="38"/>
+      <c r="B152" s="38"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="34"/>
-      <c r="B153" s="34"/>
+      <c r="A153" s="38"/>
+      <c r="B153" s="38"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="34"/>
-      <c r="B154" s="34"/>
+      <c r="A154" s="38"/>
+      <c r="B154" s="38"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="34"/>
-      <c r="B155" s="34"/>
+      <c r="A155" s="38"/>
+      <c r="B155" s="38"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="34"/>
-      <c r="B156" s="34"/>
+      <c r="A156" s="38"/>
+      <c r="B156" s="38"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="34"/>
-      <c r="B157" s="34"/>
+      <c r="A157" s="38"/>
+      <c r="B157" s="38"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="34"/>
-      <c r="B158" s="34"/>
+      <c r="A158" s="38"/>
+      <c r="B158" s="38"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="34"/>
-      <c r="B159" s="34"/>
+      <c r="A159" s="38"/>
+      <c r="B159" s="38"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="34"/>
-      <c r="B160" s="34"/>
+      <c r="A160" s="38"/>
+      <c r="B160" s="38"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="34"/>
-      <c r="B161" s="34"/>
+      <c r="A161" s="38"/>
+      <c r="B161" s="38"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="34"/>
-      <c r="B162" s="34"/>
+      <c r="A162" s="38"/>
+      <c r="B162" s="38"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="34"/>
-      <c r="B163" s="34"/>
+      <c r="A163" s="38"/>
+      <c r="B163" s="38"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="34"/>
-      <c r="B164" s="34"/>
+      <c r="A164" s="38"/>
+      <c r="B164" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="145">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A161:B161"/>
+    <mergeCell ref="A162:B162"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="A164:B164"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="A157:B157"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="A72:B72"/>
@@ -3408,96 +3466,51 @@
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A68:B68"/>
     <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="A161:B161"/>
-    <mergeCell ref="A162:B162"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="A164:B164"/>
-    <mergeCell ref="A155:B155"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="A157:B157"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3527,17 +3540,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
@@ -3611,16 +3624,16 @@
         <v>3216</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="H5" s="29" t="s">
         <v>101</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -9080,10 +9093,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD668FA6-C86B-4B15-9051-DF984B595504}">
-  <dimension ref="A1:I305"/>
+  <dimension ref="A1:I306"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9101,17 +9114,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -9147,22 +9160,22 @@
       <c r="B4" s="30"/>
       <c r="C4" s="2"/>
       <c r="D4" s="28" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="E4" s="5">
         <v>1608</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H4" s="28" t="s">
         <v>101</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -9327,7 +9340,7 @@
         <v>1632</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>590</v>
+        <v>645</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>363</v>
@@ -9339,199 +9352,191 @@
         <v>364</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>11</v>
-      </c>
-      <c r="B11" s="10">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>7</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>368</v>
-      </c>
-      <c r="E11" s="5">
-        <v>3216</v>
+    <row r="11" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+      <c r="D11" s="34" t="s">
+        <v>362</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>644</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>588</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>141</v>
+        <v>646</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>650</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B12" s="10">
         <v>0</v>
       </c>
       <c r="C12" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E12" s="5">
-        <v>1608</v>
+        <v>3216</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>565</v>
+        <v>588</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>6</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B13" s="10">
         <v>0</v>
       </c>
       <c r="C13" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>291</v>
+        <v>369</v>
       </c>
       <c r="E13" s="5">
         <v>1608</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>292</v>
+        <v>122</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>293</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B14" s="10">
         <v>0</v>
       </c>
       <c r="C14" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>370</v>
+        <v>291</v>
       </c>
       <c r="E14" s="5">
         <v>1608</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>136</v>
+        <v>292</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
-      <c r="D15" s="33" t="s">
-        <v>641</v>
+        <v>293</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>4</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>370</v>
       </c>
       <c r="E15" s="5">
         <v>1608</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>642</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>643</v>
-      </c>
-      <c r="H15" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="I15" s="33" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>42</v>
-      </c>
-      <c r="B16" s="10">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>25</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>371</v>
+        <v>567</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+      <c r="D16" s="33" t="s">
+        <v>637</v>
       </c>
       <c r="E16" s="5">
         <v>1608</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>573</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="H16" s="10" t="s">
+        <v>638</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>639</v>
+      </c>
+      <c r="H16" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="I16" s="10" t="s">
-        <v>113</v>
+      <c r="I16" s="33" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B17" s="10">
         <v>0</v>
       </c>
       <c r="C17" s="2">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>294</v>
+        <v>371</v>
       </c>
       <c r="E17" s="5">
         <v>1608</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>295</v>
+        <v>112</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>296</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -9545,267 +9550,267 @@
         <v>8</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="E18" s="5">
         <v>1608</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B19" s="10">
         <v>0</v>
       </c>
       <c r="C19" s="2">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>372</v>
+        <v>285</v>
       </c>
       <c r="E19" s="5">
         <v>1608</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>138</v>
+        <v>286</v>
       </c>
       <c r="H19" s="10" t="s">
         <v>101</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="2"/>
-      <c r="D20" s="33" t="s">
-        <v>637</v>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>16</v>
+      </c>
+      <c r="B20" s="10">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2">
+        <v>16</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>372</v>
       </c>
       <c r="E20" s="5">
         <v>1608</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>638</v>
-      </c>
-      <c r="G20" s="33" t="s">
-        <v>639</v>
-      </c>
-      <c r="H20" s="33" t="s">
+        <v>576</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="H20" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="I20" s="33" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
-        <v>4</v>
-      </c>
-      <c r="B21" s="10">
-        <v>0</v>
-      </c>
-      <c r="C21" s="2">
-        <v>4</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>373</v>
+      <c r="I20" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="2"/>
+      <c r="D21" s="33" t="s">
+        <v>633</v>
       </c>
       <c r="E21" s="5">
         <v>1608</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>568</v>
+        <v>634</v>
       </c>
       <c r="G21" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="H21" s="10" t="s">
+        <v>635</v>
+      </c>
+      <c r="H21" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="I21" s="10" t="s">
-        <v>129</v>
+      <c r="I21" s="33" t="s">
+        <v>636</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B22" s="10">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C22" s="2">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>282</v>
+        <v>373</v>
       </c>
       <c r="E22" s="5">
         <v>1608</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>569</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>283</v>
+        <v>568</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>128</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>284</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B23" s="10">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C23" s="2">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>282</v>
       </c>
       <c r="E23" s="5">
+        <v>1608</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>10</v>
+      </c>
+      <c r="B24" s="10">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>9</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="E24" s="5">
         <v>1632</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>591</v>
-      </c>
-      <c r="G23" s="10" t="s">
+      <c r="F24" s="5" t="s">
+        <v>647</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H24" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="I23" s="10" t="s">
+      <c r="I24" s="10" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="2"/>
-      <c r="D24" s="31" t="s">
-        <v>622</v>
-      </c>
-      <c r="E24" s="5">
-        <v>1608</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>623</v>
-      </c>
-      <c r="G24" s="31" t="s">
-        <v>624</v>
-      </c>
-      <c r="H24" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="I24" s="31" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
-        <v>4</v>
-      </c>
-      <c r="B25" s="10">
-        <v>0</v>
-      </c>
-      <c r="C25" s="2">
-        <v>4</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>374</v>
+    <row r="25" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="2"/>
+      <c r="D25" s="31" t="s">
+        <v>618</v>
       </c>
       <c r="E25" s="5">
         <v>1608</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>578</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H25" s="10" t="s">
+        <v>619</v>
+      </c>
+      <c r="G25" s="31" t="s">
+        <v>620</v>
+      </c>
+      <c r="H25" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="I25" s="10" t="s">
-        <v>125</v>
+      <c r="I25" s="31" t="s">
+        <v>621</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B26" s="10">
         <v>0</v>
       </c>
       <c r="C26" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E26" s="5">
         <v>1608</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>570</v>
+        <v>578</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B27" s="10">
         <v>0</v>
       </c>
       <c r="C27" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>297</v>
+        <v>375</v>
       </c>
       <c r="E27" s="5">
         <v>1608</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>298</v>
+        <v>116</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>146</v>
+        <v>6</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>299</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -9819,346 +9824,370 @@
         <v>8</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="E28" s="5">
         <v>1608</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="H28" s="10" t="s">
         <v>146</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29" s="10">
         <v>0</v>
       </c>
       <c r="C29" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>342</v>
+        <v>288</v>
       </c>
       <c r="E29" s="5">
         <v>1608</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>343</v>
+        <v>289</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>344</v>
+        <v>290</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B30" s="10">
         <v>0</v>
       </c>
       <c r="C30" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>279</v>
+        <v>342</v>
       </c>
       <c r="E30" s="5">
         <v>1608</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>572</v>
+        <v>580</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>280</v>
+        <v>343</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>281</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B31" s="10">
         <v>0</v>
       </c>
       <c r="C31" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>376</v>
+        <v>279</v>
       </c>
       <c r="E31" s="5">
         <v>1608</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>581</v>
+        <v>572</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>126</v>
+        <v>280</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>127</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" s="10">
         <v>0</v>
       </c>
       <c r="C32" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E32" s="5">
         <v>1608</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="H32" s="10" t="s">
         <v>101</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B33" s="10">
         <v>0</v>
       </c>
       <c r="C33" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E33" s="5">
         <v>1608</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="I33" s="10" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B34" s="10">
         <v>0</v>
       </c>
       <c r="C34" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E34" s="5">
         <v>1608</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B35" s="10">
         <v>0</v>
       </c>
       <c r="C35" s="2">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>237</v>
+        <v>379</v>
       </c>
       <c r="E35" s="5">
         <v>1608</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>235</v>
+        <v>132</v>
       </c>
       <c r="H35" s="10" t="s">
         <v>101</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>236</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B36" s="10">
         <v>0</v>
       </c>
       <c r="C36" s="2">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>300</v>
+        <v>237</v>
       </c>
       <c r="E36" s="5">
         <v>1608</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>577</v>
+        <v>585</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>301</v>
+        <v>235</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>302</v>
+        <v>236</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B37" s="10">
         <v>0</v>
       </c>
       <c r="C37" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>380</v>
+        <v>300</v>
       </c>
       <c r="E37" s="5">
         <v>1608</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>120</v>
+        <v>301</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>121</v>
+        <v>302</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B38" s="10">
         <v>0</v>
       </c>
       <c r="C38" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>111</v>
+        <v>380</v>
+      </c>
+      <c r="E38" s="5">
+        <v>1608</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B39" s="10">
         <v>0</v>
       </c>
       <c r="C39" s="2">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>303</v>
-      </c>
-      <c r="E39" s="5">
-        <v>1608</v>
+        <v>109</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>592</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>303</v>
+        <v>648</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="H39" s="10" t="s">
         <v>146</v>
       </c>
       <c r="I39" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>21</v>
+      </c>
+      <c r="B40" s="10">
+        <v>0</v>
+      </c>
+      <c r="C40" s="2">
+        <v>13</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="E40" s="5">
+        <v>1608</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="I40" s="10" t="s">
         <v>304</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C40" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -11486,15 +11515,20 @@
         <v>238</v>
       </c>
     </row>
+    <row r="306" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C306" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A5:I49">
-    <sortCondition ref="D5:D49"/>
-    <sortCondition ref="E5:E49"/>
+  <sortState ref="A5:I50">
+    <sortCondition ref="D5:D50"/>
+    <sortCondition ref="E5:E50"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:C305">
+  <conditionalFormatting sqref="C5:C306">
     <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -11506,6 +11540,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E11" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -11513,7 +11550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F2F944-B53A-4DFB-A96A-499E091FDAD5}">
   <dimension ref="A1:I300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
@@ -11532,17 +11569,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -11729,16 +11766,16 @@
         <v>1608</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="G9" s="33" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>6</v>
       </c>
       <c r="I9" s="33" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -13232,17 +13269,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -13510,22 +13547,22 @@
         <v>238</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>101</v>
       </c>
       <c r="I12" s="26" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -13536,19 +13573,19 @@
         <v>229</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>101</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -13559,19 +13596,19 @@
         <v>227</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>599</v>
+      </c>
+      <c r="G14" s="27" t="s">
         <v>600</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>603</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>604</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>101</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -15041,17 +15078,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
@@ -15440,22 +15477,22 @@
         <v>238</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>146</v>
       </c>
       <c r="I16" s="28" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
@@ -15463,22 +15500,22 @@
         <v>238</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="H17" s="10" t="s">
         <v>146</v>
       </c>
       <c r="I17" s="28" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
@@ -16928,17 +16965,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -17583,22 +17620,22 @@
         <v>238</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="E25" s="32" t="s">
         <v>197</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G25" s="32" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="H25" s="10" t="s">
         <v>101</v>
       </c>
       <c r="I25" s="32" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -17606,22 +17643,22 @@
         <v>238</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>314</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="G26" s="33" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="H26" s="10" t="s">
         <v>101</v>
       </c>
       <c r="I26" s="33" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -19031,17 +19068,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -19260,22 +19297,22 @@
         <v>238</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>101</v>
       </c>
       <c r="I11" s="31" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -20756,20 +20793,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
       <c r="D1" s="17"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
       <c r="D2" s="18" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Added Logic Level Shifter
</commit_message>
<xml_diff>
--- a/CougsInSpace-Inventory.xlsx
+++ b/CougsInSpace-Inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\CougsInSpace\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\GitHub\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7653A68-329E-43F7-83DC-6A38061AC49D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4AA19E-7A02-4A50-87B0-7B23245F536F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="2" activeTab="8" xr2:uid="{42A108CB-A0BE-49ED-8B7A-3FB1AB856735}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="1" activeTab="4" xr2:uid="{42A108CB-A0BE-49ED-8B7A-3FB1AB856735}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3858" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3874" uniqueCount="692">
   <si>
     <t>Vendors have been selected by high reputability and lowest price</t>
   </si>
@@ -2078,6 +2078,45 @@
   </si>
   <si>
     <t>Ground station</t>
+  </si>
+  <si>
+    <t>TXS0102DQM</t>
+  </si>
+  <si>
+    <t>TXS0102DQMR</t>
+  </si>
+  <si>
+    <t>X2SON-8</t>
+  </si>
+  <si>
+    <t>296-28435-1-ND</t>
+  </si>
+  <si>
+    <t>28-0005</t>
+  </si>
+  <si>
+    <t>4.75MΩ</t>
+  </si>
+  <si>
+    <t>CRCW06034M75FKEA</t>
+  </si>
+  <si>
+    <t>541-4.75MHCT-ND</t>
+  </si>
+  <si>
+    <t>21-4754</t>
+  </si>
+  <si>
+    <t>U.FL Receptacle</t>
+  </si>
+  <si>
+    <t>U.FL</t>
+  </si>
+  <si>
+    <t>04-0008</t>
+  </si>
+  <si>
+    <t>WM5587TR-ND</t>
   </si>
 </sst>
 </file>
@@ -2170,7 +2209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2224,15 +2263,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2621,7 +2663,7 @@
   <dimension ref="A1:J164"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="10" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="bottomLeft" activeCell="A70" sqref="A70:B70"/>
     </sheetView>
@@ -2777,732 +2819,777 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="44" t="s">
         <v>411</v>
       </c>
-      <c r="B24" s="38"/>
+      <c r="B24" s="44"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="44" t="s">
         <v>412</v>
       </c>
-      <c r="B25" s="38"/>
+      <c r="B25" s="44"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="44" t="s">
         <v>413</v>
       </c>
-      <c r="B26" s="38"/>
+      <c r="B26" s="44"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="44" t="s">
         <v>414</v>
       </c>
-      <c r="B27" s="38"/>
+      <c r="B27" s="44"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="44" t="s">
         <v>415</v>
       </c>
-      <c r="B28" s="38"/>
+      <c r="B28" s="44"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="44" t="s">
         <v>416</v>
       </c>
-      <c r="B29" s="38"/>
+      <c r="B29" s="44"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="44" t="s">
         <v>417</v>
       </c>
-      <c r="B30" s="38"/>
+      <c r="B30" s="44"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="44" t="s">
         <v>418</v>
       </c>
-      <c r="B31" s="38"/>
+      <c r="B31" s="44"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="44" t="s">
         <v>419</v>
       </c>
-      <c r="B32" s="38"/>
+      <c r="B32" s="44"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="44" t="s">
         <v>420</v>
       </c>
-      <c r="B33" s="38"/>
+      <c r="B33" s="44"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="45" t="s">
         <v>516</v>
       </c>
-      <c r="B34" s="39"/>
+      <c r="B34" s="45"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="38" t="s">
+      <c r="A35" s="44" t="s">
         <v>517</v>
       </c>
-      <c r="B35" s="38"/>
+      <c r="B35" s="44"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="44" t="s">
         <v>518</v>
       </c>
-      <c r="B36" s="38"/>
+      <c r="B36" s="44"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="38" t="s">
+      <c r="A37" s="44" t="s">
         <v>519</v>
       </c>
-      <c r="B37" s="38"/>
+      <c r="B37" s="44"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="45" t="s">
         <v>520</v>
       </c>
-      <c r="B38" s="39"/>
+      <c r="B38" s="45"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="45" t="s">
         <v>521</v>
       </c>
-      <c r="B39" s="39"/>
+      <c r="B39" s="45"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="45" t="s">
         <v>514</v>
       </c>
-      <c r="B40" s="39"/>
+      <c r="B40" s="45"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="45" t="s">
         <v>515</v>
       </c>
-      <c r="B41" s="39"/>
+      <c r="B41" s="45"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="45" t="s">
         <v>523</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="45"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="45" t="s">
         <v>527</v>
       </c>
-      <c r="B43" s="39"/>
+      <c r="B43" s="45"/>
     </row>
     <row r="44" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="40" t="s">
+      <c r="A44" s="46" t="s">
         <v>471</v>
       </c>
-      <c r="B44" s="40"/>
+      <c r="B44" s="46"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="38" t="s">
+      <c r="A45" s="44" t="s">
         <v>462</v>
       </c>
-      <c r="B45" s="38"/>
+      <c r="B45" s="44"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="38" t="s">
+      <c r="A46" s="44" t="s">
         <v>463</v>
       </c>
-      <c r="B46" s="38"/>
+      <c r="B46" s="44"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="44" t="s">
         <v>464</v>
       </c>
-      <c r="B47" s="38"/>
+      <c r="B47" s="44"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="38" t="s">
+      <c r="A48" s="44" t="s">
         <v>465</v>
       </c>
-      <c r="B48" s="38"/>
+      <c r="B48" s="44"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="38" t="s">
+      <c r="A49" s="44" t="s">
         <v>466</v>
       </c>
-      <c r="B49" s="38"/>
+      <c r="B49" s="44"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="38" t="s">
+      <c r="A50" s="44" t="s">
         <v>467</v>
       </c>
-      <c r="B50" s="38"/>
+      <c r="B50" s="44"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="38" t="s">
+      <c r="A51" s="44" t="s">
         <v>468</v>
       </c>
-      <c r="B51" s="38"/>
+      <c r="B51" s="44"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="38" t="s">
+      <c r="A52" s="44" t="s">
         <v>469</v>
       </c>
-      <c r="B52" s="38"/>
+      <c r="B52" s="44"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="38" t="s">
+      <c r="A53" s="44" t="s">
         <v>470</v>
       </c>
-      <c r="B53" s="38"/>
+      <c r="B53" s="44"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="38" t="s">
+      <c r="A54" s="44" t="s">
         <v>451</v>
       </c>
-      <c r="B54" s="38"/>
+      <c r="B54" s="44"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="38" t="s">
+      <c r="A55" s="44" t="s">
         <v>452</v>
       </c>
-      <c r="B55" s="38"/>
+      <c r="B55" s="44"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="38" t="s">
+      <c r="A56" s="44" t="s">
         <v>453</v>
       </c>
-      <c r="B56" s="38"/>
+      <c r="B56" s="44"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="39" t="s">
+      <c r="A57" s="45" t="s">
         <v>454</v>
       </c>
-      <c r="B57" s="39"/>
+      <c r="B57" s="45"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="45" t="s">
         <v>455</v>
       </c>
-      <c r="B58" s="39"/>
+      <c r="B58" s="45"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="39" t="s">
+      <c r="A59" s="45" t="s">
         <v>456</v>
       </c>
-      <c r="B59" s="39"/>
+      <c r="B59" s="45"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="39" t="s">
+      <c r="A60" s="45" t="s">
         <v>457</v>
       </c>
-      <c r="B60" s="39"/>
+      <c r="B60" s="45"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="39" t="s">
+      <c r="A61" s="45" t="s">
         <v>458</v>
       </c>
-      <c r="B61" s="39"/>
+      <c r="B61" s="45"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="38" t="s">
+      <c r="A62" s="44" t="s">
         <v>510</v>
       </c>
-      <c r="B62" s="38"/>
+      <c r="B62" s="44"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="38" t="s">
+      <c r="A63" s="44" t="s">
         <v>511</v>
       </c>
-      <c r="B63" s="38"/>
+      <c r="B63" s="44"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="38" t="s">
+      <c r="A64" s="44" t="s">
         <v>488</v>
       </c>
-      <c r="B64" s="38"/>
+      <c r="B64" s="44"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="38" t="s">
+      <c r="A65" s="44" t="s">
         <v>489</v>
       </c>
-      <c r="B65" s="38"/>
+      <c r="B65" s="44"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="38" t="s">
+      <c r="A66" s="44" t="s">
         <v>490</v>
       </c>
-      <c r="B66" s="38"/>
+      <c r="B66" s="44"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="38" t="s">
+      <c r="A67" s="44" t="s">
         <v>491</v>
       </c>
-      <c r="B67" s="38"/>
+      <c r="B67" s="44"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="38" t="s">
+      <c r="A68" s="44" t="s">
         <v>492</v>
       </c>
-      <c r="B68" s="38"/>
+      <c r="B68" s="44"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="38" t="s">
+      <c r="A69" s="44" t="s">
         <v>493</v>
       </c>
-      <c r="B69" s="38"/>
+      <c r="B69" s="44"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="38" t="s">
+      <c r="A70" s="44" t="s">
         <v>494</v>
       </c>
-      <c r="B70" s="38"/>
+      <c r="B70" s="44"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="38" t="s">
+      <c r="A71" s="44" t="s">
         <v>495</v>
       </c>
-      <c r="B71" s="38"/>
+      <c r="B71" s="44"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="38" t="s">
+      <c r="A72" s="44" t="s">
         <v>496</v>
       </c>
-      <c r="B72" s="38"/>
+      <c r="B72" s="44"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="38" t="s">
+      <c r="A73" s="44" t="s">
         <v>497</v>
       </c>
-      <c r="B73" s="38"/>
+      <c r="B73" s="44"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="39" t="s">
+      <c r="A74" s="45" t="s">
         <v>529</v>
       </c>
-      <c r="B74" s="39"/>
+      <c r="B74" s="45"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="39" t="s">
+      <c r="A75" s="45" t="s">
         <v>530</v>
       </c>
-      <c r="B75" s="39"/>
+      <c r="B75" s="45"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="39" t="s">
+      <c r="A76" s="45" t="s">
         <v>552</v>
       </c>
-      <c r="B76" s="39"/>
+      <c r="B76" s="45"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="39" t="s">
+      <c r="A77" s="45" t="s">
         <v>531</v>
       </c>
-      <c r="B77" s="39"/>
+      <c r="B77" s="45"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="39" t="s">
+      <c r="A78" s="45" t="s">
         <v>532</v>
       </c>
-      <c r="B78" s="39"/>
+      <c r="B78" s="45"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="39" t="s">
+      <c r="A79" s="45" t="s">
         <v>533</v>
       </c>
-      <c r="B79" s="39"/>
+      <c r="B79" s="45"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="39" t="s">
+      <c r="A80" s="45" t="s">
         <v>534</v>
       </c>
-      <c r="B80" s="39"/>
+      <c r="B80" s="45"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="39" t="s">
+      <c r="A81" s="45" t="s">
         <v>535</v>
       </c>
-      <c r="B81" s="39"/>
+      <c r="B81" s="45"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="38"/>
-      <c r="B82" s="38"/>
+      <c r="A82" s="44"/>
+      <c r="B82" s="44"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="38"/>
-      <c r="B83" s="38"/>
+      <c r="A83" s="44"/>
+      <c r="B83" s="44"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="38"/>
-      <c r="B84" s="38"/>
+      <c r="A84" s="44"/>
+      <c r="B84" s="44"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="38"/>
-      <c r="B85" s="38"/>
+      <c r="A85" s="44"/>
+      <c r="B85" s="44"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="38"/>
-      <c r="B86" s="38"/>
+      <c r="A86" s="44"/>
+      <c r="B86" s="44"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="38"/>
-      <c r="B87" s="38"/>
+      <c r="A87" s="44"/>
+      <c r="B87" s="44"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="38"/>
-      <c r="B88" s="38"/>
+      <c r="A88" s="44"/>
+      <c r="B88" s="44"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="38"/>
-      <c r="B89" s="38"/>
+      <c r="A89" s="44"/>
+      <c r="B89" s="44"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="38"/>
-      <c r="B90" s="38"/>
+      <c r="A90" s="44"/>
+      <c r="B90" s="44"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="38"/>
-      <c r="B91" s="38"/>
+      <c r="A91" s="44"/>
+      <c r="B91" s="44"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="38"/>
-      <c r="B92" s="38"/>
+      <c r="A92" s="44"/>
+      <c r="B92" s="44"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="38"/>
-      <c r="B93" s="38"/>
+      <c r="A93" s="44"/>
+      <c r="B93" s="44"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="38"/>
-      <c r="B94" s="38"/>
+      <c r="A94" s="44"/>
+      <c r="B94" s="44"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="38"/>
-      <c r="B95" s="38"/>
+      <c r="A95" s="44"/>
+      <c r="B95" s="44"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="38"/>
-      <c r="B96" s="38"/>
+      <c r="A96" s="44"/>
+      <c r="B96" s="44"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="38"/>
-      <c r="B97" s="38"/>
+      <c r="A97" s="44"/>
+      <c r="B97" s="44"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="38"/>
-      <c r="B98" s="38"/>
+      <c r="A98" s="44"/>
+      <c r="B98" s="44"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="38"/>
-      <c r="B99" s="38"/>
+      <c r="A99" s="44"/>
+      <c r="B99" s="44"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="38"/>
-      <c r="B100" s="38"/>
+      <c r="A100" s="44"/>
+      <c r="B100" s="44"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="38"/>
-      <c r="B101" s="38"/>
+      <c r="A101" s="44"/>
+      <c r="B101" s="44"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="38"/>
-      <c r="B102" s="38"/>
+      <c r="A102" s="44"/>
+      <c r="B102" s="44"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="38"/>
-      <c r="B103" s="38"/>
+      <c r="A103" s="44"/>
+      <c r="B103" s="44"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="38"/>
-      <c r="B104" s="38"/>
+      <c r="A104" s="44"/>
+      <c r="B104" s="44"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="38"/>
-      <c r="B105" s="38"/>
+      <c r="A105" s="44"/>
+      <c r="B105" s="44"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="38"/>
-      <c r="B106" s="38"/>
+      <c r="A106" s="44"/>
+      <c r="B106" s="44"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="38"/>
-      <c r="B107" s="38"/>
+      <c r="A107" s="44"/>
+      <c r="B107" s="44"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="38"/>
-      <c r="B108" s="38"/>
+      <c r="A108" s="44"/>
+      <c r="B108" s="44"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="38"/>
-      <c r="B109" s="38"/>
+      <c r="A109" s="44"/>
+      <c r="B109" s="44"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="38"/>
-      <c r="B110" s="38"/>
+      <c r="A110" s="44"/>
+      <c r="B110" s="44"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="38"/>
-      <c r="B111" s="38"/>
+      <c r="A111" s="44"/>
+      <c r="B111" s="44"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="38"/>
-      <c r="B112" s="38"/>
+      <c r="A112" s="44"/>
+      <c r="B112" s="44"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="38"/>
-      <c r="B113" s="38"/>
+      <c r="A113" s="44"/>
+      <c r="B113" s="44"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="38"/>
-      <c r="B114" s="38"/>
+      <c r="A114" s="44"/>
+      <c r="B114" s="44"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="38"/>
-      <c r="B115" s="38"/>
+      <c r="A115" s="44"/>
+      <c r="B115" s="44"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="38"/>
-      <c r="B116" s="38"/>
+      <c r="A116" s="44"/>
+      <c r="B116" s="44"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="38"/>
-      <c r="B117" s="38"/>
+      <c r="A117" s="44"/>
+      <c r="B117" s="44"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="38"/>
-      <c r="B118" s="38"/>
+      <c r="A118" s="44"/>
+      <c r="B118" s="44"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="38"/>
-      <c r="B119" s="38"/>
+      <c r="A119" s="44"/>
+      <c r="B119" s="44"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="38"/>
-      <c r="B120" s="38"/>
+      <c r="A120" s="44"/>
+      <c r="B120" s="44"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="38"/>
-      <c r="B121" s="38"/>
+      <c r="A121" s="44"/>
+      <c r="B121" s="44"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="38"/>
-      <c r="B122" s="38"/>
+      <c r="A122" s="44"/>
+      <c r="B122" s="44"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="38"/>
-      <c r="B123" s="38"/>
+      <c r="A123" s="44"/>
+      <c r="B123" s="44"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="38"/>
-      <c r="B124" s="38"/>
+      <c r="A124" s="44"/>
+      <c r="B124" s="44"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="38"/>
-      <c r="B125" s="38"/>
+      <c r="A125" s="44"/>
+      <c r="B125" s="44"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="38"/>
-      <c r="B126" s="38"/>
+      <c r="A126" s="44"/>
+      <c r="B126" s="44"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="38"/>
-      <c r="B127" s="38"/>
+      <c r="A127" s="44"/>
+      <c r="B127" s="44"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="38"/>
-      <c r="B128" s="38"/>
+      <c r="A128" s="44"/>
+      <c r="B128" s="44"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="38"/>
-      <c r="B129" s="38"/>
+      <c r="A129" s="44"/>
+      <c r="B129" s="44"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="38"/>
-      <c r="B130" s="38"/>
+      <c r="A130" s="44"/>
+      <c r="B130" s="44"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="38"/>
-      <c r="B131" s="38"/>
+      <c r="A131" s="44"/>
+      <c r="B131" s="44"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="38"/>
-      <c r="B132" s="38"/>
+      <c r="A132" s="44"/>
+      <c r="B132" s="44"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="38"/>
-      <c r="B133" s="38"/>
+      <c r="A133" s="44"/>
+      <c r="B133" s="44"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="38"/>
-      <c r="B134" s="38"/>
+      <c r="A134" s="44"/>
+      <c r="B134" s="44"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="38"/>
-      <c r="B135" s="38"/>
+      <c r="A135" s="44"/>
+      <c r="B135" s="44"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="38"/>
-      <c r="B136" s="38"/>
+      <c r="A136" s="44"/>
+      <c r="B136" s="44"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="38"/>
-      <c r="B137" s="38"/>
+      <c r="A137" s="44"/>
+      <c r="B137" s="44"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="38"/>
-      <c r="B138" s="38"/>
+      <c r="A138" s="44"/>
+      <c r="B138" s="44"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="38"/>
-      <c r="B139" s="38"/>
+      <c r="A139" s="44"/>
+      <c r="B139" s="44"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="38"/>
-      <c r="B140" s="38"/>
+      <c r="A140" s="44"/>
+      <c r="B140" s="44"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="38"/>
-      <c r="B141" s="38"/>
+      <c r="A141" s="44"/>
+      <c r="B141" s="44"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="38"/>
-      <c r="B142" s="38"/>
+      <c r="A142" s="44"/>
+      <c r="B142" s="44"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="38"/>
-      <c r="B143" s="38"/>
+      <c r="A143" s="44"/>
+      <c r="B143" s="44"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="38"/>
-      <c r="B144" s="38"/>
+      <c r="A144" s="44"/>
+      <c r="B144" s="44"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="38"/>
-      <c r="B145" s="38"/>
+      <c r="A145" s="44"/>
+      <c r="B145" s="44"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="38"/>
-      <c r="B146" s="38"/>
+      <c r="A146" s="44"/>
+      <c r="B146" s="44"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="38"/>
-      <c r="B147" s="38"/>
+      <c r="A147" s="44"/>
+      <c r="B147" s="44"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="38"/>
-      <c r="B148" s="38"/>
+      <c r="A148" s="44"/>
+      <c r="B148" s="44"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="38"/>
-      <c r="B149" s="38"/>
+      <c r="A149" s="44"/>
+      <c r="B149" s="44"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="38"/>
-      <c r="B150" s="38"/>
+      <c r="A150" s="44"/>
+      <c r="B150" s="44"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="38"/>
-      <c r="B151" s="38"/>
+      <c r="A151" s="44"/>
+      <c r="B151" s="44"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="38"/>
-      <c r="B152" s="38"/>
+      <c r="A152" s="44"/>
+      <c r="B152" s="44"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="38"/>
-      <c r="B153" s="38"/>
+      <c r="A153" s="44"/>
+      <c r="B153" s="44"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="38"/>
-      <c r="B154" s="38"/>
+      <c r="A154" s="44"/>
+      <c r="B154" s="44"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="38"/>
-      <c r="B155" s="38"/>
+      <c r="A155" s="44"/>
+      <c r="B155" s="44"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="38"/>
-      <c r="B156" s="38"/>
+      <c r="A156" s="44"/>
+      <c r="B156" s="44"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="38"/>
-      <c r="B157" s="38"/>
+      <c r="A157" s="44"/>
+      <c r="B157" s="44"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="38"/>
-      <c r="B158" s="38"/>
+      <c r="A158" s="44"/>
+      <c r="B158" s="44"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="38"/>
-      <c r="B159" s="38"/>
+      <c r="A159" s="44"/>
+      <c r="B159" s="44"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="38"/>
-      <c r="B160" s="38"/>
+      <c r="A160" s="44"/>
+      <c r="B160" s="44"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="38"/>
-      <c r="B161" s="38"/>
+      <c r="A161" s="44"/>
+      <c r="B161" s="44"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="38"/>
-      <c r="B162" s="38"/>
+      <c r="A162" s="44"/>
+      <c r="B162" s="44"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="38"/>
-      <c r="B163" s="38"/>
+      <c r="A163" s="44"/>
+      <c r="B163" s="44"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="38"/>
-      <c r="B164" s="38"/>
+      <c r="A164" s="44"/>
+      <c r="B164" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="145">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A161:B161"/>
+    <mergeCell ref="A162:B162"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="A164:B164"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="A157:B157"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="A72:B72"/>
@@ -3513,96 +3600,51 @@
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A68:B68"/>
     <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="A161:B161"/>
-    <mergeCell ref="A162:B162"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="A164:B164"/>
-    <mergeCell ref="A155:B155"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="A157:B157"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3629,20 +3671,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
       <c r="D1" s="17"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
       <c r="D2" s="18" t="s">
         <v>35</v>
       </c>
@@ -9670,10 +9712,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD668FA6-C86B-4B15-9051-DF984B595504}">
-  <dimension ref="A1:I307"/>
+  <dimension ref="A1:I308"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37:E38"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10564,233 +10606,249 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
-        <v>22</v>
-      </c>
-      <c r="B34" s="10">
-        <v>0</v>
-      </c>
-      <c r="C34" s="2">
-        <v>5</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>378</v>
+    <row r="34" spans="1:9" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="2"/>
+      <c r="D34" s="39" t="s">
+        <v>684</v>
       </c>
       <c r="E34" s="5">
         <v>1608</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>583</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>131</v>
+        <v>687</v>
+      </c>
+      <c r="G34" s="39" t="s">
+        <v>685</v>
+      </c>
+      <c r="H34" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="I34" s="39" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B35" s="10">
         <v>0</v>
       </c>
       <c r="C35" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E35" s="5">
         <v>1608</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B36" s="10">
         <v>0</v>
       </c>
       <c r="C36" s="2">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>237</v>
+        <v>379</v>
       </c>
       <c r="E36" s="5">
         <v>1608</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>235</v>
+        <v>132</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>101</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>236</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B37" s="10">
         <v>0</v>
       </c>
       <c r="C37" s="2">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>300</v>
+        <v>237</v>
       </c>
       <c r="E37" s="5">
         <v>1608</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>577</v>
+        <v>585</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>301</v>
+        <v>235</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="2"/>
-      <c r="D38" s="35" t="s">
-        <v>652</v>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>9</v>
+      </c>
+      <c r="B38" s="10">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2">
+        <v>8</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>300</v>
       </c>
       <c r="E38" s="5">
         <v>1608</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="G38" s="35" t="s">
-        <v>653</v>
-      </c>
-      <c r="H38" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="I38" s="35" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="10">
-        <v>5</v>
-      </c>
-      <c r="B39" s="10">
-        <v>0</v>
-      </c>
-      <c r="C39" s="2">
-        <v>4</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>380</v>
+        <v>577</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="I38" s="10" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="2"/>
+      <c r="D39" s="35" t="s">
+        <v>652</v>
       </c>
       <c r="E39" s="5">
         <v>1608</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>586</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="H39" s="10" t="s">
+        <v>655</v>
+      </c>
+      <c r="G39" s="35" t="s">
+        <v>653</v>
+      </c>
+      <c r="H39" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="I39" s="10" t="s">
-        <v>121</v>
+      <c r="I39" s="35" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B40" s="10">
         <v>0</v>
       </c>
       <c r="C40" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>111</v>
+        <v>380</v>
+      </c>
+      <c r="E40" s="5">
+        <v>1608</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>648</v>
+        <v>586</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B41" s="10">
         <v>0</v>
       </c>
       <c r="C41" s="2">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>303</v>
-      </c>
-      <c r="E41" s="5">
-        <v>1608</v>
+        <v>109</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>649</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>303</v>
+        <v>648</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="H41" s="10" t="s">
         <v>146</v>
       </c>
       <c r="I41" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
+        <v>21</v>
+      </c>
+      <c r="B42" s="10">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2">
+        <v>13</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="E42" s="5">
+        <v>1608</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="I42" s="10" t="s">
         <v>304</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C42" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -12118,15 +12176,20 @@
         <v>238</v>
       </c>
     </row>
+    <row r="308" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C308" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A5:I51">
-    <sortCondition ref="D5:D51"/>
-    <sortCondition ref="E5:E51"/>
+  <sortState ref="A5:I52">
+    <sortCondition ref="D5:D52"/>
+    <sortCondition ref="E5:E52"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:C307">
+  <conditionalFormatting sqref="C5:C308">
     <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -13848,8 +13911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C04FC45-08E6-489F-B80B-6935CE0BF902}">
   <dimension ref="A1:I300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14212,6 +14275,24 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>238</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>688</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>689</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="G15" s="5">
+        <v>734120110</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="40" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -17544,8 +17625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D526D2F0-6B58-44A3-8176-A7A0AAEF1CB8}">
   <dimension ref="A1:I300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18262,6 +18343,24 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
         <v>238</v>
+      </c>
+      <c r="D27" t="s">
+        <v>679</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>683</v>
+      </c>
+      <c r="G27" t="s">
+        <v>680</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="I27" s="38" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -21375,7 +21474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA2A076-A50B-47D4-A61C-CB3E58047008}">
   <dimension ref="A1:H300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>